<commit_message>
updated slides pdf. Added 16 key 4x4 keypad to parts list
</commit_message>
<xml_diff>
--- a/IoT_Parts.xlsx
+++ b/IoT_Parts.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10111"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IoTPa\Documents\IoT\class_slides\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/limegreen/Documents/CNM/IoT/git/class_slides/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09E04BED-88ED-4C0E-BB8E-E014278AA3F9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{900461C0-ACEE-F247-8AA4-AF4DEA688BBB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2250" yWindow="450" windowWidth="20475" windowHeight="15315" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-71860" yWindow="-1100" windowWidth="24180" windowHeight="15320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Master" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Master!$A$2:$J$117</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Master!$A$2:$J$118</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="322">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="323">
   <si>
     <t>Part</t>
   </si>
@@ -1016,6 +1016,9 @@
   </si>
   <si>
     <t>Velcro</t>
+  </si>
+  <si>
+    <t>16 key 4x4 keypad</t>
   </si>
 </sst>
 </file>
@@ -1591,30 +1594,30 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:M117"/>
+  <dimension ref="A1:M118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M48" sqref="M48"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M37" sqref="M37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.42578125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="30.42578125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="10.85546875" style="3" customWidth="1"/>
-    <col min="4" max="4" width="29.85546875" style="3" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="3"/>
+    <col min="1" max="1" width="17.5" style="3" customWidth="1"/>
+    <col min="2" max="2" width="30.5" style="3" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="29.83203125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="9.1640625" style="3"/>
     <col min="6" max="6" width="14" style="3" customWidth="1"/>
-    <col min="7" max="7" width="11.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5" style="6" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="28" style="6" customWidth="1"/>
     <col min="9" max="10" width="0" style="3" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="35.140625" style="17" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="35.1640625" style="17" hidden="1" customWidth="1"/>
     <col min="12" max="12" width="14" style="3" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="24.85546875" style="24" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="3"/>
+    <col min="13" max="13" width="24.83203125" style="24" customWidth="1"/>
+    <col min="14" max="16384" width="9.1640625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="27" t="s">
         <v>172</v>
       </c>
@@ -1631,7 +1634,7 @@
       <c r="L1" s="29"/>
       <c r="M1" s="30"/>
     </row>
-    <row r="2" spans="1:13" s="5" customFormat="1" ht="63" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" s="5" customFormat="1" ht="68" x14ac:dyDescent="0.2">
       <c r="A2" s="18" t="s">
         <v>0</v>
       </c>
@@ -1670,7 +1673,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" ht="48" x14ac:dyDescent="0.2">
       <c r="A3" s="32" t="s">
         <v>6</v>
       </c>
@@ -1710,7 +1713,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A4" s="32" t="s">
         <v>10</v>
       </c>
@@ -1750,7 +1753,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="120" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" ht="208" x14ac:dyDescent="0.2">
       <c r="A5" s="32" t="s">
         <v>16</v>
       </c>
@@ -1790,7 +1793,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" ht="80" x14ac:dyDescent="0.2">
       <c r="A6" s="32" t="s">
         <v>20</v>
       </c>
@@ -1830,7 +1833,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A7" s="32" t="s">
         <v>23</v>
       </c>
@@ -1870,7 +1873,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" ht="96" x14ac:dyDescent="0.2">
       <c r="A8" s="32" t="s">
         <v>26</v>
       </c>
@@ -1910,7 +1913,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" ht="80" x14ac:dyDescent="0.2">
       <c r="A9" s="32" t="s">
         <v>29</v>
       </c>
@@ -1950,7 +1953,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="135" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" ht="256" x14ac:dyDescent="0.2">
       <c r="A10" s="32" t="s">
         <v>32</v>
       </c>
@@ -1990,7 +1993,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" ht="80" x14ac:dyDescent="0.2">
       <c r="A11" s="32" t="s">
         <v>35</v>
       </c>
@@ -2030,7 +2033,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="120" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" ht="208" x14ac:dyDescent="0.2">
       <c r="A12" s="32" t="s">
         <v>285</v>
       </c>
@@ -2070,7 +2073,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" ht="80" x14ac:dyDescent="0.2">
       <c r="A13" s="32" t="s">
         <v>40</v>
       </c>
@@ -2110,7 +2113,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="63.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" ht="80" x14ac:dyDescent="0.2">
       <c r="A14" s="37" t="s">
         <v>43</v>
       </c>
@@ -2150,7 +2153,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" ht="80" x14ac:dyDescent="0.2">
       <c r="A15" s="32" t="s">
         <v>46</v>
       </c>
@@ -2192,7 +2195,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="102" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" ht="98" x14ac:dyDescent="0.2">
       <c r="A16" s="32" t="s">
         <v>49</v>
       </c>
@@ -2232,7 +2235,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="51" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" ht="96" x14ac:dyDescent="0.2">
       <c r="A17" s="32" t="s">
         <v>52</v>
       </c>
@@ -2272,7 +2275,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="51" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" ht="80" x14ac:dyDescent="0.2">
       <c r="A18" s="32" t="s">
         <v>55</v>
       </c>
@@ -2312,7 +2315,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:13" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" ht="84" x14ac:dyDescent="0.2">
       <c r="A19" s="32" t="s">
         <v>58</v>
       </c>
@@ -2352,7 +2355,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="20" spans="1:13" ht="51" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" ht="56" x14ac:dyDescent="0.2">
       <c r="A20" s="32" t="s">
         <v>271</v>
       </c>
@@ -2392,7 +2395,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="21" spans="1:13" ht="89.25" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" ht="84" x14ac:dyDescent="0.2">
       <c r="A21" s="32" t="s">
         <v>61</v>
       </c>
@@ -2432,7 +2435,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="1:13" ht="51" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" ht="56" x14ac:dyDescent="0.2">
       <c r="A22" s="32" t="s">
         <v>64</v>
       </c>
@@ -2472,7 +2475,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="1:13" ht="51" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" ht="56" x14ac:dyDescent="0.2">
       <c r="A23" s="32" t="s">
         <v>67</v>
       </c>
@@ -2512,7 +2515,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="24" spans="1:13" ht="150" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" ht="288" x14ac:dyDescent="0.2">
       <c r="A24" s="32" t="s">
         <v>70</v>
       </c>
@@ -2552,7 +2555,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:13" ht="135" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" ht="288" x14ac:dyDescent="0.2">
       <c r="A25" s="37" t="s">
         <v>73</v>
       </c>
@@ -2592,7 +2595,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="26" spans="1:13" ht="89.25" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" ht="98" x14ac:dyDescent="0.2">
       <c r="A26" s="37" t="s">
         <v>74</v>
       </c>
@@ -2632,7 +2635,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A27" s="32" t="s">
         <v>106</v>
       </c>
@@ -2672,7 +2675,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="28" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="32" t="s">
         <v>110</v>
       </c>
@@ -2712,7 +2715,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="37" t="s">
         <v>114</v>
       </c>
@@ -2752,7 +2755,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" ht="80" x14ac:dyDescent="0.2">
       <c r="A30" s="32" t="s">
         <v>124</v>
       </c>
@@ -2792,7 +2795,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="31" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" ht="48" x14ac:dyDescent="0.2">
       <c r="A31" s="32" t="s">
         <v>151</v>
       </c>
@@ -2832,7 +2835,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="32" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A32" s="32" t="s">
         <v>155</v>
       </c>
@@ -2872,7 +2875,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="33" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A33" s="32" t="s">
         <v>228</v>
       </c>
@@ -2912,7 +2915,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="34" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A34" s="43" t="s">
         <v>162</v>
       </c>
@@ -2952,7 +2955,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="35" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A35" s="43" t="s">
         <v>162</v>
       </c>
@@ -2992,7 +2995,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="36" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" ht="96" x14ac:dyDescent="0.2">
       <c r="A36" s="43" t="s">
         <v>273</v>
       </c>
@@ -3027,7 +3030,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:13" ht="135" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" ht="240" x14ac:dyDescent="0.2">
       <c r="A37" s="43" t="s">
         <v>280</v>
       </c>
@@ -3060,7 +3063,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="43" t="s">
         <v>178</v>
       </c>
@@ -3100,7 +3103,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="39" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13" ht="112" x14ac:dyDescent="0.2">
       <c r="A39" s="44" t="s">
         <v>182</v>
       </c>
@@ -3140,7 +3143,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="40" spans="1:13" ht="126" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:13" ht="119" x14ac:dyDescent="0.2">
       <c r="A40" s="43" t="s">
         <v>262</v>
       </c>
@@ -3180,7 +3183,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="41" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A41" s="46" t="s">
         <v>304</v>
       </c>
@@ -3199,7 +3202,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="42" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" s="46" t="s">
         <v>305</v>
       </c>
@@ -3218,7 +3221,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="43" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A43" s="46" t="s">
         <v>306</v>
       </c>
@@ -3237,67 +3240,49 @@
         <v>8</v>
       </c>
     </row>
-    <row r="44" spans="1:13" ht="195" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A44" s="46" t="s">
-        <v>307</v>
-      </c>
-      <c r="B44" s="44" t="s">
-        <v>308</v>
-      </c>
-      <c r="C44" s="48" t="s">
-        <v>18</v>
-      </c>
-      <c r="D44" s="49" t="s">
-        <v>309</v>
-      </c>
-      <c r="E44" s="48">
-        <v>9.99</v>
-      </c>
-      <c r="F44" s="48">
-        <v>2</v>
-      </c>
-      <c r="G44" s="34">
-        <f t="shared" ref="G44:G45" si="4">E44*F44</f>
-        <v>19.98</v>
-      </c>
-      <c r="H44" s="50">
-        <f>G44</f>
-        <v>19.98</v>
-      </c>
+        <v>322</v>
+      </c>
+      <c r="B44" s="47"/>
+      <c r="C44" s="48"/>
+      <c r="D44" s="49"/>
+      <c r="E44" s="48"/>
+      <c r="F44" s="48"/>
+      <c r="G44" s="50"/>
+      <c r="H44" s="50"/>
       <c r="I44" s="10"/>
       <c r="J44" s="9"/>
       <c r="K44" s="32"/>
       <c r="L44" s="32"/>
-      <c r="M44" s="23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:13" ht="105" x14ac:dyDescent="0.25">
+      <c r="M44" s="23"/>
+    </row>
+    <row r="45" spans="1:13" ht="208" x14ac:dyDescent="0.2">
       <c r="A45" s="46" t="s">
-        <v>313</v>
+        <v>307</v>
       </c>
       <c r="B45" s="44" t="s">
-        <v>316</v>
+        <v>308</v>
       </c>
       <c r="C45" s="48" t="s">
         <v>18</v>
       </c>
       <c r="D45" s="49" t="s">
-        <v>315</v>
+        <v>309</v>
       </c>
       <c r="E45" s="48">
-        <v>36.99</v>
+        <v>9.99</v>
       </c>
       <c r="F45" s="48">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G45" s="34">
-        <f t="shared" si="4"/>
-        <v>36.99</v>
+        <f t="shared" ref="G45:G46" si="4">E45*F45</f>
+        <v>19.98</v>
       </c>
       <c r="H45" s="50">
         <f>G45</f>
-        <v>36.99</v>
+        <v>19.98</v>
       </c>
       <c r="I45" s="10"/>
       <c r="J45" s="9"/>
@@ -3307,32 +3292,32 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:13" ht="270" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:13" ht="112" x14ac:dyDescent="0.2">
       <c r="A46" s="46" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B46" s="44" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C46" s="48" t="s">
         <v>18</v>
       </c>
       <c r="D46" s="49" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="E46" s="48">
-        <v>15.96</v>
+        <v>36.99</v>
       </c>
       <c r="F46" s="48">
         <v>1</v>
       </c>
       <c r="G46" s="34">
-        <f t="shared" ref="G46" si="5">E46*F46</f>
-        <v>15.96</v>
+        <f t="shared" si="4"/>
+        <v>36.99</v>
       </c>
       <c r="H46" s="50">
         <f>G46</f>
-        <v>15.96</v>
+        <v>36.99</v>
       </c>
       <c r="I46" s="10"/>
       <c r="J46" s="9"/>
@@ -3342,32 +3327,32 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:13" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:13" ht="256" x14ac:dyDescent="0.2">
       <c r="A47" s="46" t="s">
-        <v>321</v>
+        <v>314</v>
       </c>
       <c r="B47" s="44" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="C47" s="48" t="s">
         <v>18</v>
       </c>
       <c r="D47" s="49" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="E47" s="48">
-        <v>15.25</v>
+        <v>15.96</v>
       </c>
       <c r="F47" s="48">
         <v>1</v>
       </c>
       <c r="G47" s="34">
-        <f t="shared" ref="G47" si="6">E47*F47</f>
-        <v>15.25</v>
+        <f t="shared" ref="G47" si="5">E47*F47</f>
+        <v>15.96</v>
       </c>
       <c r="H47" s="50">
         <f>G47</f>
-        <v>15.25</v>
+        <v>15.96</v>
       </c>
       <c r="I47" s="10"/>
       <c r="J47" s="9"/>
@@ -3377,22 +3362,42 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A48" s="46"/>
-      <c r="B48" s="47"/>
-      <c r="C48" s="48"/>
-      <c r="D48" s="49"/>
-      <c r="E48" s="48"/>
-      <c r="F48" s="48"/>
-      <c r="G48" s="50"/>
-      <c r="H48" s="50"/>
+    <row r="48" spans="1:13" ht="85" x14ac:dyDescent="0.2">
+      <c r="A48" s="46" t="s">
+        <v>321</v>
+      </c>
+      <c r="B48" s="44" t="s">
+        <v>319</v>
+      </c>
+      <c r="C48" s="48" t="s">
+        <v>18</v>
+      </c>
+      <c r="D48" s="49" t="s">
+        <v>320</v>
+      </c>
+      <c r="E48" s="48">
+        <v>15.25</v>
+      </c>
+      <c r="F48" s="48">
+        <v>1</v>
+      </c>
+      <c r="G48" s="34">
+        <f t="shared" ref="G48" si="6">E48*F48</f>
+        <v>15.25</v>
+      </c>
+      <c r="H48" s="50">
+        <f>G48</f>
+        <v>15.25</v>
+      </c>
       <c r="I48" s="10"/>
       <c r="J48" s="9"/>
       <c r="K48" s="32"/>
       <c r="L48" s="32"/>
-      <c r="M48" s="23"/>
-    </row>
-    <row r="49" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="M48" s="23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A49" s="46"/>
       <c r="B49" s="47"/>
       <c r="C49" s="48"/>
@@ -3407,7 +3412,7 @@
       <c r="L49" s="32"/>
       <c r="M49" s="23"/>
     </row>
-    <row r="50" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A50" s="46"/>
       <c r="B50" s="47"/>
       <c r="C50" s="48"/>
@@ -3422,7 +3427,7 @@
       <c r="L50" s="32"/>
       <c r="M50" s="23"/>
     </row>
-    <row r="51" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A51" s="46"/>
       <c r="B51" s="47"/>
       <c r="C51" s="48"/>
@@ -3437,71 +3442,71 @@
       <c r="L51" s="32"/>
       <c r="M51" s="23"/>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A52" s="32"/>
-      <c r="B52" s="32"/>
-      <c r="C52" s="32"/>
-      <c r="D52" s="32"/>
-      <c r="E52" s="32"/>
-      <c r="F52" s="32"/>
-      <c r="G52" s="34"/>
-      <c r="H52" s="34"/>
+    <row r="52" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="A52" s="46"/>
+      <c r="B52" s="47"/>
+      <c r="C52" s="48"/>
+      <c r="D52" s="49"/>
+      <c r="E52" s="48"/>
+      <c r="F52" s="48"/>
+      <c r="G52" s="50"/>
+      <c r="H52" s="50"/>
       <c r="I52" s="10"/>
       <c r="J52" s="9"/>
       <c r="K52" s="32"/>
       <c r="L52" s="32"/>
-      <c r="M52" s="26"/>
-    </row>
-    <row r="53" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A53" s="32" t="s">
-        <v>185</v>
-      </c>
-      <c r="B53" s="32" t="s">
-        <v>186</v>
-      </c>
+      <c r="M52" s="23"/>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A53" s="32"/>
+      <c r="B53" s="32"/>
       <c r="C53" s="32"/>
       <c r="D53" s="32"/>
-      <c r="E53" s="32">
-        <v>25</v>
-      </c>
-      <c r="F53" s="32">
-        <v>16</v>
-      </c>
-      <c r="G53" s="34">
-        <f t="shared" ref="G53" si="7">E53*F53</f>
-        <v>400</v>
-      </c>
-      <c r="H53" s="34">
-        <f t="shared" ref="H53" si="8">0.75*G53</f>
-        <v>300</v>
-      </c>
-      <c r="I53" s="7">
-        <v>0</v>
-      </c>
-      <c r="J53" s="9">
-        <f t="shared" ref="J53" si="9">I53*E53</f>
-        <v>0</v>
-      </c>
+      <c r="E53" s="32"/>
+      <c r="F53" s="32"/>
+      <c r="G53" s="34"/>
+      <c r="H53" s="34"/>
+      <c r="I53" s="10"/>
+      <c r="J53" s="9"/>
       <c r="K53" s="32"/>
       <c r="L53" s="32"/>
       <c r="M53" s="26"/>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A54" s="32"/>
-      <c r="B54" s="32"/>
+    <row r="54" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="A54" s="32" t="s">
+        <v>185</v>
+      </c>
+      <c r="B54" s="32" t="s">
+        <v>186</v>
+      </c>
       <c r="C54" s="32"/>
       <c r="D54" s="32"/>
-      <c r="E54" s="32"/>
-      <c r="F54" s="32"/>
-      <c r="G54" s="34"/>
-      <c r="H54" s="34"/>
-      <c r="I54" s="7"/>
-      <c r="J54" s="9"/>
+      <c r="E54" s="32">
+        <v>25</v>
+      </c>
+      <c r="F54" s="32">
+        <v>16</v>
+      </c>
+      <c r="G54" s="34">
+        <f t="shared" ref="G54" si="7">E54*F54</f>
+        <v>400</v>
+      </c>
+      <c r="H54" s="34">
+        <f t="shared" ref="H54" si="8">0.75*G54</f>
+        <v>300</v>
+      </c>
+      <c r="I54" s="7">
+        <v>0</v>
+      </c>
+      <c r="J54" s="9">
+        <f t="shared" ref="J54" si="9">I54*E54</f>
+        <v>0</v>
+      </c>
       <c r="K54" s="32"/>
       <c r="L54" s="32"/>
       <c r="M54" s="26"/>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A55" s="32"/>
       <c r="B55" s="32"/>
       <c r="C55" s="32"/>
@@ -3516,35 +3521,24 @@
       <c r="L55" s="32"/>
       <c r="M55" s="26"/>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A56" s="32" t="s">
-        <v>171</v>
-      </c>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A56" s="32"/>
       <c r="B56" s="32"/>
       <c r="C56" s="32"/>
       <c r="D56" s="32"/>
       <c r="E56" s="32"/>
       <c r="F56" s="32"/>
-      <c r="G56" s="34">
-        <f>SUM(G3:G55)</f>
-        <v>5488.4900000000016</v>
-      </c>
-      <c r="H56" s="34">
-        <f>SUM(H3:H55)</f>
-        <v>4310.4025000000001</v>
-      </c>
+      <c r="G56" s="34"/>
+      <c r="H56" s="34"/>
       <c r="I56" s="7"/>
-      <c r="J56" s="9">
-        <f>SUM(J3:J55)</f>
-        <v>3098.7799999999993</v>
-      </c>
+      <c r="J56" s="9"/>
       <c r="K56" s="32"/>
       <c r="L56" s="32"/>
       <c r="M56" s="26"/>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A57" s="32" t="s">
-        <v>187</v>
+        <v>171</v>
       </c>
       <c r="B57" s="32"/>
       <c r="C57" s="32"/>
@@ -3552,161 +3546,150 @@
       <c r="E57" s="32"/>
       <c r="F57" s="32"/>
       <c r="G57" s="34">
-        <f>G56/16</f>
-        <v>343.0306250000001</v>
+        <f>SUM(G3:G56)</f>
+        <v>5488.4900000000016</v>
       </c>
       <c r="H57" s="34">
-        <f>0.75*G57</f>
-        <v>257.27296875000008</v>
+        <f>SUM(H3:H56)</f>
+        <v>4310.4025000000001</v>
       </c>
       <c r="I57" s="7"/>
-      <c r="J57" s="9"/>
+      <c r="J57" s="9">
+        <f>SUM(J3:J56)</f>
+        <v>3098.7799999999993</v>
+      </c>
       <c r="K57" s="32"/>
       <c r="L57" s="32"/>
       <c r="M57" s="26"/>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A58" s="27" t="s">
-        <v>188</v>
-      </c>
-      <c r="B58" s="27"/>
-      <c r="C58" s="27"/>
-      <c r="D58" s="27"/>
-      <c r="E58" s="27"/>
-      <c r="F58" s="27"/>
-      <c r="G58" s="27"/>
-      <c r="H58" s="27"/>
-      <c r="I58" s="27"/>
-      <c r="J58" s="27"/>
+    <row r="58" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="A58" s="32" t="s">
+        <v>187</v>
+      </c>
+      <c r="B58" s="32"/>
+      <c r="C58" s="32"/>
+      <c r="D58" s="32"/>
+      <c r="E58" s="32"/>
+      <c r="F58" s="32"/>
+      <c r="G58" s="34">
+        <f>G57/16</f>
+        <v>343.0306250000001</v>
+      </c>
+      <c r="H58" s="34">
+        <f>0.75*G58</f>
+        <v>257.27296875000008</v>
+      </c>
+      <c r="I58" s="7"/>
+      <c r="J58" s="9"/>
       <c r="K58" s="32"/>
       <c r="L58" s="32"/>
-      <c r="M58" s="27"/>
-    </row>
-    <row r="59" spans="1:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="A59" s="31" t="s">
-        <v>0</v>
-      </c>
-      <c r="B59" s="31" t="s">
-        <v>1</v>
-      </c>
-      <c r="C59" s="31" t="s">
-        <v>2</v>
-      </c>
-      <c r="D59" s="31" t="s">
-        <v>3</v>
-      </c>
-      <c r="E59" s="31" t="s">
-        <v>4</v>
-      </c>
-      <c r="F59" s="45" t="s">
-        <v>189</v>
-      </c>
-      <c r="G59" s="34"/>
-      <c r="H59" s="32"/>
-      <c r="I59" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="J59" s="9"/>
+      <c r="M58" s="26"/>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A59" s="27" t="s">
+        <v>188</v>
+      </c>
+      <c r="B59" s="27"/>
+      <c r="C59" s="27"/>
+      <c r="D59" s="27"/>
+      <c r="E59" s="27"/>
+      <c r="F59" s="27"/>
+      <c r="G59" s="27"/>
+      <c r="H59" s="27"/>
+      <c r="I59" s="27"/>
+      <c r="J59" s="27"/>
       <c r="K59" s="32"/>
       <c r="L59" s="32"/>
-      <c r="M59" s="26"/>
-    </row>
-    <row r="60" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A60" s="37" t="s">
-        <v>13</v>
-      </c>
-      <c r="B60" s="37" t="s">
-        <v>14</v>
-      </c>
-      <c r="C60" s="37" t="s">
-        <v>8</v>
-      </c>
-      <c r="D60" s="39" t="s">
-        <v>15</v>
-      </c>
-      <c r="E60" s="37">
-        <v>24.95</v>
-      </c>
-      <c r="F60" s="37">
+      <c r="M59" s="27"/>
+    </row>
+    <row r="60" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+      <c r="A60" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="B60" s="31" t="s">
+        <v>1</v>
+      </c>
+      <c r="C60" s="31" t="s">
+        <v>2</v>
+      </c>
+      <c r="D60" s="31" t="s">
+        <v>3</v>
+      </c>
+      <c r="E60" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="F60" s="45" t="s">
+        <v>189</v>
+      </c>
+      <c r="G60" s="34"/>
+      <c r="H60" s="32"/>
+      <c r="I60" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="G60" s="40">
-        <f t="shared" ref="G60:G96" si="10">E60*F60</f>
-        <v>124.75</v>
-      </c>
-      <c r="H60" s="37"/>
-      <c r="I60" s="8">
-        <v>1</v>
-      </c>
-      <c r="J60" s="9">
-        <f t="shared" ref="J60:J83" si="11">I60*E60</f>
-        <v>24.95</v>
-      </c>
+      <c r="J60" s="9"/>
       <c r="K60" s="32"/>
       <c r="L60" s="32"/>
-      <c r="M60" s="26">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="61" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A61" s="32" t="s">
-        <v>77</v>
-      </c>
-      <c r="B61" s="35" t="s">
-        <v>78</v>
-      </c>
-      <c r="C61" s="35" t="s">
-        <v>18</v>
-      </c>
-      <c r="D61" s="36" t="s">
-        <v>79</v>
-      </c>
-      <c r="E61" s="32">
-        <v>172.77</v>
-      </c>
-      <c r="F61" s="32">
+      <c r="M60" s="26"/>
+    </row>
+    <row r="61" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+      <c r="A61" s="37" t="s">
+        <v>13</v>
+      </c>
+      <c r="B61" s="37" t="s">
+        <v>14</v>
+      </c>
+      <c r="C61" s="37" t="s">
+        <v>8</v>
+      </c>
+      <c r="D61" s="39" t="s">
+        <v>15</v>
+      </c>
+      <c r="E61" s="37">
+        <v>24.95</v>
+      </c>
+      <c r="F61" s="37">
+        <v>5</v>
+      </c>
+      <c r="G61" s="40">
+        <f t="shared" ref="G61:G97" si="10">E61*F61</f>
+        <v>124.75</v>
+      </c>
+      <c r="H61" s="37"/>
+      <c r="I61" s="8">
         <v>1</v>
       </c>
-      <c r="G61" s="34">
-        <f t="shared" si="10"/>
-        <v>172.77</v>
-      </c>
-      <c r="H61" s="32"/>
-      <c r="I61" s="8">
-        <v>0</v>
-      </c>
       <c r="J61" s="9">
-        <f t="shared" si="11"/>
-        <v>0</v>
+        <f t="shared" ref="J61:J84" si="11">I61*E61</f>
+        <v>24.95</v>
       </c>
       <c r="K61" s="32"/>
       <c r="L61" s="32"/>
       <c r="M61" s="26">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" ht="28" x14ac:dyDescent="0.2">
+      <c r="A62" s="32" t="s">
+        <v>77</v>
+      </c>
+      <c r="B62" s="35" t="s">
+        <v>78</v>
+      </c>
+      <c r="C62" s="35" t="s">
+        <v>18</v>
+      </c>
+      <c r="D62" s="36" t="s">
+        <v>79</v>
+      </c>
+      <c r="E62" s="32">
+        <v>172.77</v>
+      </c>
+      <c r="F62" s="32">
         <v>1</v>
-      </c>
-    </row>
-    <row r="62" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A62" s="32" t="s">
-        <v>80</v>
-      </c>
-      <c r="B62" s="35" t="s">
-        <v>81</v>
-      </c>
-      <c r="C62" s="35" t="s">
-        <v>18</v>
-      </c>
-      <c r="D62" s="36" t="s">
-        <v>82</v>
-      </c>
-      <c r="E62" s="32">
-        <v>17.98</v>
-      </c>
-      <c r="F62" s="32">
-        <v>4</v>
       </c>
       <c r="G62" s="34">
         <f t="shared" si="10"/>
-        <v>71.92</v>
+        <v>172.77</v>
       </c>
       <c r="H62" s="32"/>
       <c r="I62" s="8">
@@ -3719,31 +3702,31 @@
       <c r="K62" s="32"/>
       <c r="L62" s="32"/>
       <c r="M62" s="26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="A63" s="32" t="s">
+        <v>80</v>
+      </c>
+      <c r="B63" s="35" t="s">
+        <v>81</v>
+      </c>
+      <c r="C63" s="35" t="s">
+        <v>18</v>
+      </c>
+      <c r="D63" s="36" t="s">
+        <v>82</v>
+      </c>
+      <c r="E63" s="32">
+        <v>17.98</v>
+      </c>
+      <c r="F63" s="32">
         <v>4</v>
-      </c>
-    </row>
-    <row r="63" spans="1:13" ht="120" x14ac:dyDescent="0.25">
-      <c r="A63" s="32" t="s">
-        <v>83</v>
-      </c>
-      <c r="B63" s="32" t="s">
-        <v>84</v>
-      </c>
-      <c r="C63" s="32" t="s">
-        <v>18</v>
-      </c>
-      <c r="D63" s="36" t="s">
-        <v>85</v>
-      </c>
-      <c r="E63" s="32">
-        <v>15.99</v>
-      </c>
-      <c r="F63" s="32">
-        <v>3</v>
       </c>
       <c r="G63" s="34">
         <f t="shared" si="10"/>
-        <v>47.97</v>
+        <v>71.92</v>
       </c>
       <c r="H63" s="32"/>
       <c r="I63" s="8">
@@ -3755,101 +3738,101 @@
       </c>
       <c r="K63" s="32"/>
       <c r="L63" s="32"/>
-      <c r="M63" s="23" t="s">
+      <c r="M63" s="26">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" ht="112" x14ac:dyDescent="0.2">
+      <c r="A64" s="32" t="s">
+        <v>83</v>
+      </c>
+      <c r="B64" s="32" t="s">
+        <v>84</v>
+      </c>
+      <c r="C64" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="D64" s="36" t="s">
+        <v>85</v>
+      </c>
+      <c r="E64" s="32">
+        <v>15.99</v>
+      </c>
+      <c r="F64" s="32">
+        <v>3</v>
+      </c>
+      <c r="G64" s="34">
+        <f t="shared" si="10"/>
+        <v>47.97</v>
+      </c>
+      <c r="H64" s="32"/>
+      <c r="I64" s="8">
+        <v>0</v>
+      </c>
+      <c r="J64" s="9">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="K64" s="32"/>
+      <c r="L64" s="32"/>
+      <c r="M64" s="23" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="64" spans="1:13" ht="90" x14ac:dyDescent="0.25">
-      <c r="A64" s="51" t="s">
+    <row r="65" spans="1:13" ht="80" x14ac:dyDescent="0.2">
+      <c r="A65" s="51" t="s">
         <v>310</v>
       </c>
-      <c r="B64" s="51" t="s">
+      <c r="B65" s="51" t="s">
         <v>312</v>
       </c>
-      <c r="C64" s="51" t="s">
-        <v>18</v>
-      </c>
-      <c r="D64" s="52" t="s">
+      <c r="C65" s="51" t="s">
+        <v>18</v>
+      </c>
+      <c r="D65" s="52" t="s">
         <v>311</v>
       </c>
-      <c r="E64" s="51">
+      <c r="E65" s="51">
         <v>7.19</v>
       </c>
-      <c r="F64" s="51">
+      <c r="F65" s="51">
         <v>4</v>
       </c>
-      <c r="G64" s="53">
+      <c r="G65" s="53">
         <f t="shared" si="10"/>
         <v>28.76</v>
       </c>
-      <c r="H64" s="51"/>
-      <c r="I64" s="8"/>
-      <c r="J64" s="9"/>
-      <c r="K64" s="32"/>
-      <c r="L64" s="32"/>
-      <c r="M64" s="23">
+      <c r="H65" s="51"/>
+      <c r="I65" s="8"/>
+      <c r="J65" s="9"/>
+      <c r="K65" s="32"/>
+      <c r="L65" s="32"/>
+      <c r="M65" s="23">
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:13" ht="105" x14ac:dyDescent="0.25">
-      <c r="A65" s="32" t="s">
+    <row r="66" spans="1:13" ht="96" x14ac:dyDescent="0.2">
+      <c r="A66" s="32" t="s">
         <v>86</v>
       </c>
-      <c r="B65" s="32" t="s">
+      <c r="B66" s="32" t="s">
         <v>87</v>
       </c>
-      <c r="C65" s="32" t="s">
-        <v>18</v>
-      </c>
-      <c r="D65" s="33" t="s">
+      <c r="C66" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="D66" s="33" t="s">
         <v>88</v>
       </c>
-      <c r="E65" s="32">
+      <c r="E66" s="32">
         <v>11.98</v>
       </c>
-      <c r="F65" s="32">
+      <c r="F66" s="32">
         <v>1</v>
       </c>
-      <c r="G65" s="34">
+      <c r="G66" s="34">
         <f t="shared" si="10"/>
         <v>11.98</v>
-      </c>
-      <c r="H65" s="32"/>
-      <c r="I65" s="8">
-        <v>0</v>
-      </c>
-      <c r="J65" s="9">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="K65" s="32"/>
-      <c r="L65" s="32"/>
-      <c r="M65" s="26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66" spans="1:13" ht="60" x14ac:dyDescent="0.25">
-      <c r="A66" s="32" t="s">
-        <v>89</v>
-      </c>
-      <c r="B66" s="32" t="s">
-        <v>90</v>
-      </c>
-      <c r="C66" s="32" t="s">
-        <v>18</v>
-      </c>
-      <c r="D66" s="36" t="s">
-        <v>91</v>
-      </c>
-      <c r="E66" s="32">
-        <v>94.99</v>
-      </c>
-      <c r="F66" s="32">
-        <v>4</v>
-      </c>
-      <c r="G66" s="34">
-        <f t="shared" si="10"/>
-        <v>379.96</v>
       </c>
       <c r="H66" s="32"/>
       <c r="I66" s="8">
@@ -3862,31 +3845,31 @@
       <c r="K66" s="32"/>
       <c r="L66" s="32"/>
       <c r="M66" s="26">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="67" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:13" ht="48" x14ac:dyDescent="0.2">
       <c r="A67" s="32" t="s">
-        <v>117</v>
+        <v>89</v>
       </c>
       <c r="B67" s="32" t="s">
-        <v>117</v>
+        <v>90</v>
       </c>
       <c r="C67" s="32" t="s">
-        <v>112</v>
+        <v>18</v>
       </c>
       <c r="D67" s="36" t="s">
-        <v>118</v>
+        <v>91</v>
       </c>
       <c r="E67" s="32">
-        <v>149.99</v>
+        <v>94.99</v>
       </c>
       <c r="F67" s="32">
         <v>4</v>
       </c>
       <c r="G67" s="34">
         <f t="shared" si="10"/>
-        <v>599.96</v>
+        <v>379.96</v>
       </c>
       <c r="H67" s="32"/>
       <c r="I67" s="8">
@@ -3902,28 +3885,28 @@
         <v>4</v>
       </c>
     </row>
-    <row r="68" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A68" s="32" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B68" s="32" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C68" s="32" t="s">
         <v>112</v>
       </c>
       <c r="D68" s="36" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="E68" s="32">
-        <v>99.99</v>
+        <v>149.99</v>
       </c>
       <c r="F68" s="32">
         <v>4</v>
       </c>
       <c r="G68" s="34">
         <f t="shared" si="10"/>
-        <v>399.96</v>
+        <v>599.96</v>
       </c>
       <c r="H68" s="32"/>
       <c r="I68" s="8">
@@ -3939,102 +3922,102 @@
         <v>4</v>
       </c>
     </row>
-    <row r="69" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A69" s="37" t="s">
-        <v>121</v>
-      </c>
-      <c r="B69" s="38" t="s">
-        <v>122</v>
-      </c>
-      <c r="C69" s="38" t="s">
+    <row r="69" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+      <c r="A69" s="32" t="s">
+        <v>119</v>
+      </c>
+      <c r="B69" s="32" t="s">
+        <v>119</v>
+      </c>
+      <c r="C69" s="32" t="s">
         <v>112</v>
       </c>
-      <c r="D69" s="42" t="s">
-        <v>123</v>
-      </c>
-      <c r="E69" s="37">
-        <v>149.99</v>
-      </c>
-      <c r="F69" s="37">
-        <v>1</v>
-      </c>
-      <c r="G69" s="40">
+      <c r="D69" s="36" t="s">
+        <v>120</v>
+      </c>
+      <c r="E69" s="32">
+        <v>99.99</v>
+      </c>
+      <c r="F69" s="32">
+        <v>4</v>
+      </c>
+      <c r="G69" s="34">
         <f t="shared" si="10"/>
-        <v>149.99</v>
-      </c>
-      <c r="H69" s="40"/>
+        <v>399.96</v>
+      </c>
+      <c r="H69" s="32"/>
       <c r="I69" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J69" s="9">
         <f t="shared" si="11"/>
-        <v>149.99</v>
+        <v>0</v>
       </c>
       <c r="K69" s="32"/>
       <c r="L69" s="32"/>
       <c r="M69" s="26">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="70" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A70" s="32" t="s">
-        <v>128</v>
-      </c>
-      <c r="B70" s="35" t="s">
-        <v>129</v>
-      </c>
-      <c r="C70" s="35" t="s">
-        <v>130</v>
-      </c>
-      <c r="D70" s="36" t="s">
-        <v>131</v>
-      </c>
-      <c r="E70" s="32">
-        <v>15.95</v>
-      </c>
-      <c r="F70" s="32">
-        <v>18</v>
-      </c>
-      <c r="G70" s="34">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="70" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="A70" s="37" t="s">
+        <v>121</v>
+      </c>
+      <c r="B70" s="38" t="s">
+        <v>122</v>
+      </c>
+      <c r="C70" s="38" t="s">
+        <v>112</v>
+      </c>
+      <c r="D70" s="42" t="s">
+        <v>123</v>
+      </c>
+      <c r="E70" s="37">
+        <v>149.99</v>
+      </c>
+      <c r="F70" s="37">
+        <v>1</v>
+      </c>
+      <c r="G70" s="40">
         <f t="shared" si="10"/>
-        <v>287.09999999999997</v>
-      </c>
-      <c r="H70" s="32"/>
+        <v>149.99</v>
+      </c>
+      <c r="H70" s="40"/>
       <c r="I70" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J70" s="9">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>149.99</v>
       </c>
       <c r="K70" s="32"/>
       <c r="L70" s="32"/>
       <c r="M70" s="26">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="71" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="71" spans="1:13" ht="28" x14ac:dyDescent="0.2">
       <c r="A71" s="32" t="s">
-        <v>132</v>
-      </c>
-      <c r="B71" s="32" t="s">
-        <v>133</v>
-      </c>
-      <c r="C71" s="32" t="s">
+        <v>128</v>
+      </c>
+      <c r="B71" s="35" t="s">
+        <v>129</v>
+      </c>
+      <c r="C71" s="35" t="s">
         <v>130</v>
       </c>
-      <c r="D71" s="33" t="s">
-        <v>134</v>
+      <c r="D71" s="36" t="s">
+        <v>131</v>
       </c>
       <c r="E71" s="32">
-        <v>110.9</v>
+        <v>15.95</v>
       </c>
       <c r="F71" s="32">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="G71" s="34">
         <f t="shared" si="10"/>
-        <v>554.5</v>
+        <v>287.09999999999997</v>
       </c>
       <c r="H71" s="32"/>
       <c r="I71" s="8">
@@ -4047,31 +4030,31 @@
       <c r="K71" s="32"/>
       <c r="L71" s="32"/>
       <c r="M71" s="26">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="72" spans="1:13" ht="38.25" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="72" spans="1:13" ht="80" x14ac:dyDescent="0.2">
       <c r="A72" s="32" t="s">
-        <v>190</v>
-      </c>
-      <c r="B72" s="35" t="s">
-        <v>191</v>
-      </c>
-      <c r="C72" s="35" t="s">
+        <v>132</v>
+      </c>
+      <c r="B72" s="32" t="s">
+        <v>133</v>
+      </c>
+      <c r="C72" s="32" t="s">
         <v>130</v>
       </c>
-      <c r="D72" s="36" t="s">
-        <v>192</v>
+      <c r="D72" s="33" t="s">
+        <v>134</v>
       </c>
       <c r="E72" s="32">
-        <v>57.95</v>
+        <v>110.9</v>
       </c>
       <c r="F72" s="32">
         <v>5</v>
       </c>
       <c r="G72" s="34">
         <f t="shared" si="10"/>
-        <v>289.75</v>
+        <v>554.5</v>
       </c>
       <c r="H72" s="32"/>
       <c r="I72" s="8">
@@ -4087,28 +4070,28 @@
         <v>5</v>
       </c>
     </row>
-    <row r="73" spans="1:13" ht="51" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:13" ht="42" x14ac:dyDescent="0.2">
       <c r="A73" s="32" t="s">
-        <v>135</v>
+        <v>190</v>
       </c>
       <c r="B73" s="35" t="s">
-        <v>136</v>
+        <v>191</v>
       </c>
       <c r="C73" s="35" t="s">
         <v>130</v>
       </c>
       <c r="D73" s="36" t="s">
-        <v>137</v>
+        <v>192</v>
       </c>
       <c r="E73" s="32">
-        <v>52.95</v>
+        <v>57.95</v>
       </c>
       <c r="F73" s="32">
         <v>5</v>
       </c>
       <c r="G73" s="34">
         <f t="shared" si="10"/>
-        <v>264.75</v>
+        <v>289.75</v>
       </c>
       <c r="H73" s="32"/>
       <c r="I73" s="8">
@@ -4124,36 +4107,36 @@
         <v>5</v>
       </c>
     </row>
-    <row r="74" spans="1:13" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:13" ht="56" x14ac:dyDescent="0.2">
       <c r="A74" s="32" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="B74" s="35" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="C74" s="35" t="s">
         <v>130</v>
       </c>
       <c r="D74" s="36" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="E74" s="32">
-        <v>42.95</v>
+        <v>52.95</v>
       </c>
       <c r="F74" s="32">
         <v>5</v>
       </c>
       <c r="G74" s="34">
         <f t="shared" si="10"/>
-        <v>214.75</v>
+        <v>264.75</v>
       </c>
       <c r="H74" s="32"/>
       <c r="I74" s="8">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J74" s="9">
         <f t="shared" si="11"/>
-        <v>85.9</v>
+        <v>0</v>
       </c>
       <c r="K74" s="32"/>
       <c r="L74" s="32"/>
@@ -4161,36 +4144,36 @@
         <v>5</v>
       </c>
     </row>
-    <row r="75" spans="1:13" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:13" ht="42" x14ac:dyDescent="0.2">
       <c r="A75" s="32" t="s">
-        <v>193</v>
+        <v>141</v>
       </c>
       <c r="B75" s="35" t="s">
-        <v>194</v>
+        <v>142</v>
       </c>
       <c r="C75" s="35" t="s">
         <v>130</v>
       </c>
       <c r="D75" s="36" t="s">
-        <v>195</v>
+        <v>143</v>
       </c>
       <c r="E75" s="32">
-        <v>25.95</v>
+        <v>42.95</v>
       </c>
       <c r="F75" s="32">
         <v>5</v>
       </c>
       <c r="G75" s="34">
         <f t="shared" si="10"/>
-        <v>129.75</v>
+        <v>214.75</v>
       </c>
       <c r="H75" s="32"/>
       <c r="I75" s="8">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J75" s="9">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>85.9</v>
       </c>
       <c r="K75" s="32"/>
       <c r="L75" s="32"/>
@@ -4198,28 +4181,28 @@
         <v>5</v>
       </c>
     </row>
-    <row r="76" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:13" ht="42" x14ac:dyDescent="0.2">
       <c r="A76" s="32" t="s">
-        <v>196</v>
-      </c>
-      <c r="B76" s="32" t="s">
-        <v>197</v>
-      </c>
-      <c r="C76" s="32" t="s">
+        <v>193</v>
+      </c>
+      <c r="B76" s="35" t="s">
+        <v>194</v>
+      </c>
+      <c r="C76" s="35" t="s">
         <v>130</v>
       </c>
-      <c r="D76" s="33" t="s">
-        <v>198</v>
+      <c r="D76" s="36" t="s">
+        <v>195</v>
       </c>
       <c r="E76" s="32">
-        <v>22.95</v>
+        <v>25.95</v>
       </c>
       <c r="F76" s="32">
         <v>5</v>
       </c>
       <c r="G76" s="34">
         <f t="shared" si="10"/>
-        <v>114.75</v>
+        <v>129.75</v>
       </c>
       <c r="H76" s="32"/>
       <c r="I76" s="8">
@@ -4235,28 +4218,28 @@
         <v>5</v>
       </c>
     </row>
-    <row r="77" spans="1:13" ht="51" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:13" ht="64" x14ac:dyDescent="0.2">
       <c r="A77" s="32" t="s">
-        <v>138</v>
-      </c>
-      <c r="B77" s="35" t="s">
-        <v>139</v>
+        <v>196</v>
+      </c>
+      <c r="B77" s="32" t="s">
+        <v>197</v>
       </c>
       <c r="C77" s="32" t="s">
         <v>130</v>
       </c>
       <c r="D77" s="33" t="s">
-        <v>140</v>
+        <v>198</v>
       </c>
       <c r="E77" s="32">
-        <v>27.95</v>
+        <v>22.95</v>
       </c>
       <c r="F77" s="32">
         <v>5</v>
       </c>
       <c r="G77" s="34">
         <f t="shared" si="10"/>
-        <v>139.75</v>
+        <v>114.75</v>
       </c>
       <c r="H77" s="32"/>
       <c r="I77" s="8">
@@ -4272,28 +4255,28 @@
         <v>5</v>
       </c>
     </row>
-    <row r="78" spans="1:13" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:13" ht="64" x14ac:dyDescent="0.2">
       <c r="A78" s="32" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B78" s="35" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C78" s="32" t="s">
         <v>130</v>
       </c>
       <c r="D78" s="33" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="E78" s="32">
-        <v>42.95</v>
+        <v>27.95</v>
       </c>
       <c r="F78" s="32">
         <v>5</v>
       </c>
       <c r="G78" s="34">
         <f t="shared" si="10"/>
-        <v>214.75</v>
+        <v>139.75</v>
       </c>
       <c r="H78" s="32"/>
       <c r="I78" s="8">
@@ -4309,36 +4292,36 @@
         <v>5</v>
       </c>
     </row>
-    <row r="79" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:13" ht="48" x14ac:dyDescent="0.2">
       <c r="A79" s="32" t="s">
-        <v>147</v>
-      </c>
-      <c r="B79" s="32" t="s">
-        <v>148</v>
+        <v>141</v>
+      </c>
+      <c r="B79" s="35" t="s">
+        <v>142</v>
       </c>
       <c r="C79" s="32" t="s">
-        <v>149</v>
+        <v>130</v>
       </c>
       <c r="D79" s="33" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="E79" s="32">
-        <v>29.9</v>
+        <v>42.95</v>
       </c>
       <c r="F79" s="32">
         <v>5</v>
       </c>
       <c r="G79" s="34">
         <f t="shared" si="10"/>
-        <v>149.5</v>
+        <v>214.75</v>
       </c>
       <c r="H79" s="32"/>
       <c r="I79" s="8">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J79" s="9">
         <f t="shared" si="11"/>
-        <v>59.8</v>
+        <v>0</v>
       </c>
       <c r="K79" s="32"/>
       <c r="L79" s="32"/>
@@ -4346,36 +4329,36 @@
         <v>5</v>
       </c>
     </row>
-    <row r="80" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A80" s="32" t="s">
-        <v>92</v>
+        <v>147</v>
       </c>
       <c r="B80" s="32" t="s">
-        <v>93</v>
-      </c>
-      <c r="C80" s="35" t="s">
-        <v>18</v>
-      </c>
-      <c r="D80" s="36" t="s">
-        <v>94</v>
+        <v>148</v>
+      </c>
+      <c r="C80" s="32" t="s">
+        <v>149</v>
+      </c>
+      <c r="D80" s="33" t="s">
+        <v>150</v>
       </c>
       <c r="E80" s="32">
-        <v>57.8</v>
+        <v>29.9</v>
       </c>
       <c r="F80" s="32">
         <v>5</v>
       </c>
       <c r="G80" s="34">
         <f t="shared" si="10"/>
-        <v>289</v>
+        <v>149.5</v>
       </c>
       <c r="H80" s="32"/>
       <c r="I80" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J80" s="9">
         <f t="shared" si="11"/>
-        <v>57.8</v>
+        <v>59.8</v>
       </c>
       <c r="K80" s="32"/>
       <c r="L80" s="32"/>
@@ -4383,65 +4366,65 @@
         <v>5</v>
       </c>
     </row>
-    <row r="81" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A81" s="32" t="s">
-        <v>199</v>
-      </c>
-      <c r="B81" s="44" t="s">
-        <v>200</v>
+        <v>92</v>
+      </c>
+      <c r="B81" s="32" t="s">
+        <v>93</v>
       </c>
       <c r="C81" s="35" t="s">
-        <v>201</v>
-      </c>
-      <c r="D81" s="33" t="s">
-        <v>202</v>
+        <v>18</v>
+      </c>
+      <c r="D81" s="36" t="s">
+        <v>94</v>
       </c>
       <c r="E81" s="32">
-        <v>259</v>
+        <v>57.8</v>
       </c>
       <c r="F81" s="32">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="G81" s="34">
         <f t="shared" si="10"/>
-        <v>2072</v>
+        <v>289</v>
       </c>
       <c r="H81" s="32"/>
       <c r="I81" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J81" s="9">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>57.8</v>
       </c>
       <c r="K81" s="32"/>
       <c r="L81" s="32"/>
       <c r="M81" s="26">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="82" spans="1:13" ht="96" x14ac:dyDescent="0.2">
+      <c r="A82" s="32" t="s">
+        <v>199</v>
+      </c>
+      <c r="B82" s="44" t="s">
+        <v>200</v>
+      </c>
+      <c r="C82" s="35" t="s">
+        <v>201</v>
+      </c>
+      <c r="D82" s="33" t="s">
+        <v>202</v>
+      </c>
+      <c r="E82" s="32">
+        <v>259</v>
+      </c>
+      <c r="F82" s="32">
         <v>8</v>
-      </c>
-    </row>
-    <row r="82" spans="1:13" ht="94.5" x14ac:dyDescent="0.25">
-      <c r="A82" s="44" t="s">
-        <v>203</v>
-      </c>
-      <c r="B82" s="44" t="s">
-        <v>204</v>
-      </c>
-      <c r="C82" s="44" t="s">
-        <v>18</v>
-      </c>
-      <c r="D82" s="33" t="s">
-        <v>205</v>
-      </c>
-      <c r="E82" s="32">
-        <v>89.99</v>
-      </c>
-      <c r="F82" s="32">
-        <v>2</v>
       </c>
       <c r="G82" s="34">
         <f t="shared" si="10"/>
-        <v>179.98</v>
+        <v>2072</v>
       </c>
       <c r="H82" s="32"/>
       <c r="I82" s="8">
@@ -4454,31 +4437,31 @@
       <c r="K82" s="32"/>
       <c r="L82" s="32"/>
       <c r="M82" s="26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="83" spans="1:13" ht="126" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="83" spans="1:13" ht="112" x14ac:dyDescent="0.2">
       <c r="A83" s="44" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="B83" s="44" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="C83" s="44" t="s">
         <v>18</v>
       </c>
       <c r="D83" s="33" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="E83" s="32">
-        <v>21.98</v>
+        <v>89.99</v>
       </c>
       <c r="F83" s="32">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="G83" s="34">
         <f t="shared" si="10"/>
-        <v>351.68</v>
+        <v>179.98</v>
       </c>
       <c r="H83" s="32"/>
       <c r="I83" s="8">
@@ -4490,109 +4473,109 @@
       </c>
       <c r="K83" s="32"/>
       <c r="L83" s="32"/>
-      <c r="M83" s="23" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="84" spans="1:13" ht="110.25" x14ac:dyDescent="0.25">
+      <c r="M83" s="26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:13" ht="136" x14ac:dyDescent="0.2">
       <c r="A84" s="44" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="B84" s="44" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="C84" s="44" t="s">
         <v>18</v>
       </c>
       <c r="D84" s="33" t="s">
-        <v>211</v>
-      </c>
-      <c r="E84" s="44">
-        <v>12.99</v>
+        <v>208</v>
+      </c>
+      <c r="E84" s="32">
+        <v>21.98</v>
       </c>
       <c r="F84" s="32">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="G84" s="34">
         <f t="shared" si="10"/>
-        <v>64.95</v>
+        <v>351.68</v>
       </c>
       <c r="H84" s="32"/>
       <c r="I84" s="8">
         <v>0</v>
       </c>
       <c r="J84" s="9">
-        <f t="shared" ref="J84:J91" si="12">I84*E84</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="K84" s="32"/>
       <c r="L84" s="32"/>
-      <c r="M84" s="26">
+      <c r="M84" s="23" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="85" spans="1:13" ht="102" x14ac:dyDescent="0.2">
+      <c r="A85" s="44" t="s">
+        <v>209</v>
+      </c>
+      <c r="B85" s="44" t="s">
+        <v>210</v>
+      </c>
+      <c r="C85" s="44" t="s">
+        <v>18</v>
+      </c>
+      <c r="D85" s="33" t="s">
+        <v>211</v>
+      </c>
+      <c r="E85" s="44">
+        <v>12.99</v>
+      </c>
+      <c r="F85" s="32">
         <v>5</v>
-      </c>
-    </row>
-    <row r="85" spans="1:13" ht="63" x14ac:dyDescent="0.25">
-      <c r="A85" s="44" t="s">
-        <v>212</v>
-      </c>
-      <c r="B85" s="44" t="s">
-        <v>213</v>
-      </c>
-      <c r="C85" s="44" t="s">
-        <v>18</v>
-      </c>
-      <c r="D85" s="33" t="s">
-        <v>214</v>
-      </c>
-      <c r="E85" s="44">
-        <v>22.95</v>
-      </c>
-      <c r="F85" s="32">
-        <v>4</v>
       </c>
       <c r="G85" s="34">
         <f t="shared" si="10"/>
-        <v>91.8</v>
+        <v>64.95</v>
       </c>
       <c r="H85" s="32"/>
       <c r="I85" s="8">
         <v>0</v>
       </c>
       <c r="J85" s="9">
-        <f t="shared" si="12"/>
+        <f t="shared" ref="J85:J92" si="12">I85*E85</f>
         <v>0</v>
       </c>
       <c r="K85" s="32"/>
       <c r="L85" s="32"/>
       <c r="M85" s="26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="86" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="86" spans="1:13" ht="80" x14ac:dyDescent="0.2">
       <c r="A86" s="44" t="s">
         <v>212</v>
       </c>
       <c r="B86" s="44" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C86" s="44" t="s">
         <v>18</v>
       </c>
       <c r="D86" s="33" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="E86" s="44">
-        <v>49.95</v>
+        <v>22.95</v>
       </c>
       <c r="F86" s="32">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G86" s="34">
         <f t="shared" si="10"/>
-        <v>49.95</v>
+        <v>91.8</v>
       </c>
       <c r="H86" s="32"/>
-      <c r="I86" s="10">
+      <c r="I86" s="8">
         <v>0</v>
       </c>
       <c r="J86" s="9">
@@ -4605,18 +4588,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:13" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:13" ht="112" x14ac:dyDescent="0.2">
       <c r="A87" s="44" t="s">
-        <v>247</v>
+        <v>212</v>
       </c>
       <c r="B87" s="44" t="s">
-        <v>249</v>
+        <v>215</v>
       </c>
       <c r="C87" s="44" t="s">
-        <v>248</v>
+        <v>18</v>
       </c>
       <c r="D87" s="33" t="s">
-        <v>252</v>
+        <v>216</v>
       </c>
       <c r="E87" s="44">
         <v>49.95</v>
@@ -4630,11 +4613,11 @@
       </c>
       <c r="H87" s="32"/>
       <c r="I87" s="10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J87" s="9">
         <f t="shared" si="12"/>
-        <v>49.95</v>
+        <v>0</v>
       </c>
       <c r="K87" s="32"/>
       <c r="L87" s="32"/>
@@ -4642,18 +4625,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:13" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:13" ht="64" x14ac:dyDescent="0.2">
       <c r="A88" s="44" t="s">
         <v>247</v>
       </c>
       <c r="B88" s="44" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C88" s="44" t="s">
         <v>248</v>
       </c>
       <c r="D88" s="33" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="E88" s="44">
         <v>49.95</v>
@@ -4679,18 +4662,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:13" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:13" ht="64" x14ac:dyDescent="0.2">
       <c r="A89" s="44" t="s">
         <v>247</v>
       </c>
       <c r="B89" s="44" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="C89" s="44" t="s">
         <v>248</v>
       </c>
       <c r="D89" s="33" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="E89" s="44">
         <v>49.95</v>
@@ -4716,65 +4699,65 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:13" ht="110.25" x14ac:dyDescent="0.25">
-      <c r="A90" s="32" t="s">
-        <v>217</v>
+    <row r="90" spans="1:13" ht="64" x14ac:dyDescent="0.2">
+      <c r="A90" s="44" t="s">
+        <v>247</v>
       </c>
       <c r="B90" s="44" t="s">
-        <v>218</v>
-      </c>
-      <c r="C90" s="32" t="s">
-        <v>18</v>
+        <v>254</v>
+      </c>
+      <c r="C90" s="44" t="s">
+        <v>248</v>
       </c>
       <c r="D90" s="33" t="s">
-        <v>219</v>
-      </c>
-      <c r="E90" s="32">
-        <v>16.5</v>
+        <v>253</v>
+      </c>
+      <c r="E90" s="44">
+        <v>49.95</v>
       </c>
       <c r="F90" s="32">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="G90" s="34">
         <f t="shared" si="10"/>
-        <v>99</v>
+        <v>49.95</v>
       </c>
       <c r="H90" s="32"/>
       <c r="I90" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J90" s="9">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>49.95</v>
       </c>
       <c r="K90" s="32"/>
       <c r="L90" s="32"/>
-      <c r="M90" s="23" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="91" spans="1:13" ht="63" x14ac:dyDescent="0.25">
+      <c r="M90" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:13" ht="119" x14ac:dyDescent="0.2">
       <c r="A91" s="32" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="B91" s="44" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="C91" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="D91" s="36" t="s">
-        <v>222</v>
+      <c r="D91" s="33" t="s">
+        <v>219</v>
       </c>
       <c r="E91" s="32">
-        <v>12</v>
+        <v>16.5</v>
       </c>
       <c r="F91" s="32">
         <v>6</v>
       </c>
       <c r="G91" s="34">
         <f t="shared" si="10"/>
-        <v>72</v>
+        <v>99</v>
       </c>
       <c r="H91" s="32"/>
       <c r="I91" s="10">
@@ -4787,193 +4770,222 @@
       <c r="K91" s="32"/>
       <c r="L91" s="32"/>
       <c r="M91" s="23" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="92" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="92" spans="1:13" ht="51" x14ac:dyDescent="0.2">
       <c r="A92" s="32" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="B92" s="44" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="C92" s="32" t="s">
-        <v>225</v>
-      </c>
-      <c r="D92" s="33" t="s">
-        <v>226</v>
+        <v>18</v>
+      </c>
+      <c r="D92" s="36" t="s">
+        <v>222</v>
       </c>
       <c r="E92" s="32">
-        <v>0.16</v>
+        <v>12</v>
       </c>
       <c r="F92" s="32">
-        <v>100</v>
+        <v>6</v>
       </c>
       <c r="G92" s="34">
         <f t="shared" si="10"/>
-        <v>16</v>
+        <v>72</v>
       </c>
       <c r="H92" s="32"/>
       <c r="I92" s="10">
         <v>0</v>
       </c>
       <c r="J92" s="9">
-        <f t="shared" ref="J92:J95" si="13">I92*E92</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="K92" s="32"/>
       <c r="L92" s="32"/>
-      <c r="M92" s="26">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="93" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+      <c r="M92" s="23" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="93" spans="1:13" ht="176" x14ac:dyDescent="0.2">
       <c r="A93" s="32" t="s">
-        <v>257</v>
+        <v>223</v>
       </c>
       <c r="B93" s="44" t="s">
-        <v>255</v>
+        <v>224</v>
       </c>
       <c r="C93" s="32" t="s">
-        <v>18</v>
+        <v>225</v>
       </c>
       <c r="D93" s="33" t="s">
-        <v>256</v>
+        <v>226</v>
       </c>
       <c r="E93" s="32">
-        <v>18.989999999999998</v>
+        <v>0.16</v>
       </c>
       <c r="F93" s="32">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="G93" s="34">
         <f t="shared" si="10"/>
-        <v>18.989999999999998</v>
+        <v>16</v>
       </c>
       <c r="H93" s="32"/>
       <c r="I93" s="10">
-        <v>1</v>
-      </c>
-      <c r="J93" s="11">
-        <f t="shared" si="13"/>
-        <v>18.989999999999998</v>
+        <v>0</v>
+      </c>
+      <c r="J93" s="9">
+        <f t="shared" ref="J93:J96" si="13">I93*E93</f>
+        <v>0</v>
       </c>
       <c r="K93" s="32"/>
       <c r="L93" s="32"/>
       <c r="M93" s="26">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="94" spans="1:13" ht="112" x14ac:dyDescent="0.2">
+      <c r="A94" s="32" t="s">
+        <v>257</v>
+      </c>
+      <c r="B94" s="44" t="s">
+        <v>255</v>
+      </c>
+      <c r="C94" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="D94" s="33" t="s">
+        <v>256</v>
+      </c>
+      <c r="E94" s="32">
+        <v>18.989999999999998</v>
+      </c>
+      <c r="F94" s="32">
         <v>1</v>
-      </c>
-    </row>
-    <row r="94" spans="1:13" ht="150" x14ac:dyDescent="0.25">
-      <c r="A94" s="32" t="s">
-        <v>283</v>
-      </c>
-      <c r="B94" s="44" t="s">
-        <v>284</v>
-      </c>
-      <c r="C94" s="32" t="s">
-        <v>18</v>
-      </c>
-      <c r="D94" s="33" t="s">
-        <v>282</v>
-      </c>
-      <c r="E94" s="32">
-        <v>12.99</v>
-      </c>
-      <c r="F94" s="32">
-        <v>4</v>
       </c>
       <c r="G94" s="34">
         <f t="shared" si="10"/>
-        <v>51.96</v>
+        <v>18.989999999999998</v>
       </c>
       <c r="H94" s="32"/>
-      <c r="I94" s="10"/>
-      <c r="J94" s="11"/>
+      <c r="I94" s="10">
+        <v>1</v>
+      </c>
+      <c r="J94" s="11">
+        <f t="shared" si="13"/>
+        <v>18.989999999999998</v>
+      </c>
       <c r="K94" s="32"/>
       <c r="L94" s="32"/>
       <c r="M94" s="26">
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:13" ht="135" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:13" ht="272" x14ac:dyDescent="0.2">
       <c r="A95" s="32" t="s">
-        <v>260</v>
+        <v>283</v>
       </c>
       <c r="B95" s="44" t="s">
-        <v>259</v>
+        <v>284</v>
       </c>
       <c r="C95" s="32" t="s">
         <v>18</v>
       </c>
       <c r="D95" s="33" t="s">
-        <v>258</v>
+        <v>282</v>
       </c>
       <c r="E95" s="32">
-        <v>9.99</v>
+        <v>12.99</v>
       </c>
       <c r="F95" s="32">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G95" s="34">
         <f t="shared" si="10"/>
-        <v>9.99</v>
+        <v>51.96</v>
       </c>
       <c r="H95" s="32"/>
-      <c r="I95" s="10">
-        <v>1</v>
-      </c>
-      <c r="J95" s="11">
-        <f t="shared" si="13"/>
-        <v>9.99</v>
-      </c>
+      <c r="I95" s="10"/>
+      <c r="J95" s="11"/>
       <c r="K95" s="32"/>
       <c r="L95" s="32"/>
       <c r="M95" s="26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="96" spans="1:13" ht="63" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:13" ht="256" x14ac:dyDescent="0.2">
       <c r="A96" s="32" t="s">
-        <v>276</v>
+        <v>260</v>
       </c>
       <c r="B96" s="44" t="s">
-        <v>278</v>
+        <v>259</v>
       </c>
       <c r="C96" s="32" t="s">
         <v>18</v>
       </c>
       <c r="D96" s="33" t="s">
-        <v>277</v>
+        <v>258</v>
       </c>
       <c r="E96" s="32">
-        <v>8.59</v>
+        <v>9.99</v>
       </c>
       <c r="F96" s="32">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G96" s="34">
         <f t="shared" si="10"/>
-        <v>17.18</v>
+        <v>9.99</v>
       </c>
       <c r="H96" s="32"/>
-      <c r="I96" s="10"/>
-      <c r="J96" s="11"/>
+      <c r="I96" s="10">
+        <v>1</v>
+      </c>
+      <c r="J96" s="11">
+        <f t="shared" si="13"/>
+        <v>9.99</v>
+      </c>
       <c r="K96" s="32"/>
       <c r="L96" s="32"/>
       <c r="M96" s="26">
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B97" s="14"/>
-      <c r="D97" s="4"/>
-      <c r="H97" s="3"/>
-      <c r="I97" s="15"/>
-      <c r="J97" s="16"/>
-      <c r="K97" s="3"/>
-    </row>
-    <row r="98" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:13" ht="96" x14ac:dyDescent="0.2">
+      <c r="A97" s="32" t="s">
+        <v>276</v>
+      </c>
+      <c r="B97" s="44" t="s">
+        <v>278</v>
+      </c>
+      <c r="C97" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="D97" s="33" t="s">
+        <v>277</v>
+      </c>
+      <c r="E97" s="32">
+        <v>8.59</v>
+      </c>
+      <c r="F97" s="32">
+        <v>2</v>
+      </c>
+      <c r="G97" s="34">
+        <f t="shared" si="10"/>
+        <v>17.18</v>
+      </c>
+      <c r="H97" s="32"/>
+      <c r="I97" s="10"/>
+      <c r="J97" s="11"/>
+      <c r="K97" s="32"/>
+      <c r="L97" s="32"/>
+      <c r="M97" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="B98" s="14"/>
       <c r="D98" s="4"/>
       <c r="H98" s="3"/>
@@ -4981,111 +4993,89 @@
       <c r="J98" s="16"/>
       <c r="K98" s="3"/>
     </row>
-    <row r="99" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="B99" s="14"/>
+      <c r="D99" s="4"/>
       <c r="H99" s="3"/>
       <c r="I99" s="15"/>
       <c r="J99" s="16"/>
       <c r="K99" s="3"/>
     </row>
-    <row r="100" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:13" x14ac:dyDescent="0.2">
       <c r="H100" s="3"/>
-      <c r="I100" s="10" t="s">
+      <c r="I100" s="15"/>
+      <c r="J100" s="16"/>
+      <c r="K100" s="3"/>
+    </row>
+    <row r="101" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="H101" s="3"/>
+      <c r="I101" s="10" t="s">
         <v>171</v>
       </c>
-      <c r="J100" s="11">
-        <f>SUM(J60:J99)</f>
+      <c r="J101" s="11">
+        <f>SUM(J61:J100)</f>
         <v>557.2700000000001</v>
       </c>
-      <c r="K100" s="3"/>
-    </row>
-    <row r="101" spans="1:13" x14ac:dyDescent="0.25">
       <c r="K101" s="3"/>
     </row>
-    <row r="102" spans="1:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="A102" s="12" t="s">
+    <row r="102" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="K102" s="3"/>
+    </row>
+    <row r="103" spans="1:13" ht="48" x14ac:dyDescent="0.2">
+      <c r="A103" s="12" t="s">
         <v>227</v>
       </c>
-      <c r="B102" s="12"/>
-      <c r="C102" s="12"/>
-      <c r="D102" s="12"/>
-      <c r="E102" s="12"/>
-      <c r="F102" s="12"/>
-      <c r="G102" s="12"/>
-      <c r="H102" s="12"/>
-      <c r="I102" s="12"/>
-      <c r="J102" s="12"/>
-      <c r="K102" s="3"/>
-      <c r="M102" s="25"/>
-    </row>
-    <row r="103" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A103" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B103" s="5" t="s">
+      <c r="B103" s="12"/>
+      <c r="C103" s="12"/>
+      <c r="D103" s="12"/>
+      <c r="E103" s="12"/>
+      <c r="F103" s="12"/>
+      <c r="G103" s="12"/>
+      <c r="H103" s="12"/>
+      <c r="I103" s="12"/>
+      <c r="J103" s="12"/>
+      <c r="K103" s="3"/>
+      <c r="M103" s="25"/>
+    </row>
+    <row r="104" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+      <c r="A104" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B104" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C103" s="5"/>
-      <c r="D103" s="5" t="s">
+      <c r="C104" s="5"/>
+      <c r="D104" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E103" s="5" t="s">
+      <c r="E104" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="H103" s="3"/>
-      <c r="I103" s="7" t="s">
+      <c r="H104" s="3"/>
+      <c r="I104" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="J103" s="9"/>
-      <c r="K103" s="3"/>
-    </row>
-    <row r="104" spans="1:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="A104" s="3" t="s">
+      <c r="J104" s="9"/>
+      <c r="K104" s="3"/>
+    </row>
+    <row r="105" spans="1:13" ht="80" x14ac:dyDescent="0.2">
+      <c r="A105" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="B104" s="2" t="s">
+      <c r="B105" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="C104" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D104" s="4" t="s">
+      <c r="C105" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D105" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="E104" s="3">
+      <c r="E105" s="3">
         <v>23.95</v>
       </c>
-      <c r="G104" s="6">
-        <f>E104*F104</f>
-        <v>0</v>
-      </c>
-      <c r="H104" s="3"/>
-      <c r="I104" s="8">
-        <v>0</v>
-      </c>
-      <c r="J104" s="9">
-        <f>I104*E104</f>
-        <v>0</v>
-      </c>
-      <c r="K104" s="3"/>
-    </row>
-    <row r="105" spans="1:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="A105" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="B105" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="C105" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D105" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="E105" s="3">
-        <v>15.99</v>
-      </c>
       <c r="G105" s="6">
-        <f t="shared" ref="G105:G112" si="14">E105*F105</f>
+        <f>E105*F105</f>
         <v>0</v>
       </c>
       <c r="H105" s="3"/>
@@ -5093,112 +5083,112 @@
         <v>0</v>
       </c>
       <c r="J105" s="9">
-        <f t="shared" ref="J105:J117" si="15">I105*E105</f>
+        <f>I105*E105</f>
         <v>0</v>
       </c>
       <c r="K105" s="3"/>
     </row>
-    <row r="106" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:13" ht="80" x14ac:dyDescent="0.2">
       <c r="A106" s="3" t="s">
-        <v>167</v>
+        <v>98</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>168</v>
+        <v>99</v>
       </c>
       <c r="C106" s="3" t="s">
-        <v>169</v>
+        <v>18</v>
       </c>
       <c r="D106" s="4" t="s">
-        <v>170</v>
+        <v>100</v>
       </c>
       <c r="E106" s="3">
-        <v>19.95</v>
+        <v>15.99</v>
       </c>
       <c r="G106" s="6">
-        <f t="shared" si="14"/>
+        <f t="shared" ref="G106:G113" si="14">E106*F106</f>
         <v>0</v>
       </c>
       <c r="H106" s="3"/>
       <c r="I106" s="8">
+        <v>0</v>
+      </c>
+      <c r="J106" s="9">
+        <f t="shared" ref="J106:J118" si="15">I106*E106</f>
+        <v>0</v>
+      </c>
+      <c r="K106" s="3"/>
+    </row>
+    <row r="107" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+      <c r="A107" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="B107" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="C107" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="D107" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="E107" s="3">
+        <v>19.95</v>
+      </c>
+      <c r="G107" s="6">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="H107" s="3"/>
+      <c r="I107" s="8">
         <v>10</v>
       </c>
-      <c r="J106" s="9">
+      <c r="J107" s="9">
         <f t="shared" si="15"/>
         <v>199.5</v>
       </c>
-      <c r="K106" s="3"/>
-    </row>
-    <row r="107" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A107" s="3" t="s">
+      <c r="K107" s="3"/>
+    </row>
+    <row r="108" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+      <c r="A108" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B107" s="3" t="s">
+      <c r="B108" s="3" t="s">
         <v>265</v>
       </c>
-      <c r="C107" s="3" t="s">
+      <c r="C108" s="3" t="s">
         <v>169</v>
       </c>
-      <c r="D107" s="1" t="s">
+      <c r="D108" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="E107" s="3">
+      <c r="E108" s="3">
         <v>4.95</v>
       </c>
-      <c r="H107" s="3"/>
-      <c r="I107" s="8">
+      <c r="H108" s="3"/>
+      <c r="I108" s="8">
         <v>5</v>
       </c>
-      <c r="J107" s="9">
+      <c r="J108" s="9">
         <f t="shared" si="15"/>
         <v>24.75</v>
       </c>
-      <c r="K107" s="3"/>
-    </row>
-    <row r="108" spans="1:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="A108" s="3" t="s">
+      <c r="K108" s="3"/>
+    </row>
+    <row r="109" spans="1:13" ht="48" x14ac:dyDescent="0.2">
+      <c r="A109" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="B108" s="3" t="s">
+      <c r="B109" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C108" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D108" s="1" t="s">
+      <c r="C109" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D109" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="E108" s="3">
+      <c r="E109" s="3">
         <v>10.98</v>
-      </c>
-      <c r="G108" s="6">
-        <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
-      <c r="H108" s="3"/>
-      <c r="I108" s="8">
-        <v>0</v>
-      </c>
-      <c r="J108" s="9">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
-      <c r="K108" s="3"/>
-    </row>
-    <row r="109" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A109" s="3" t="s">
-        <v>228</v>
-      </c>
-      <c r="B109" s="3" t="s">
-        <v>229</v>
-      </c>
-      <c r="C109" s="3" t="s">
-        <v>230</v>
-      </c>
-      <c r="D109" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="E109" s="3">
-        <v>7.95</v>
       </c>
       <c r="G109" s="6">
         <f t="shared" si="14"/>
@@ -5206,84 +5196,84 @@
       </c>
       <c r="H109" s="3"/>
       <c r="I109" s="8">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="J109" s="9">
         <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="K109" s="3"/>
+    </row>
+    <row r="110" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+      <c r="A110" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="B110" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="C110" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="D110" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="E110" s="3">
+        <v>7.95</v>
+      </c>
+      <c r="G110" s="6">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="H110" s="3"/>
+      <c r="I110" s="8">
+        <v>16</v>
+      </c>
+      <c r="J110" s="9">
+        <f t="shared" si="15"/>
         <v>127.2</v>
       </c>
-      <c r="K109" s="3"/>
-    </row>
-    <row r="110" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A110" s="3" t="s">
+      <c r="K110" s="3"/>
+    </row>
+    <row r="111" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+      <c r="A111" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="B110" s="3" t="s">
+      <c r="B111" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="C110" s="3" t="s">
+      <c r="C111" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="D110" s="4" t="s">
+      <c r="D111" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="E110" s="3">
+      <c r="E111" s="3">
         <v>3.5</v>
       </c>
-      <c r="I110" s="10">
-        <v>0</v>
-      </c>
-      <c r="J110" s="9">
-        <f>I110*E110</f>
-        <v>0</v>
-      </c>
-      <c r="K110" s="3"/>
-    </row>
-    <row r="111" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A111" s="3" t="s">
+      <c r="I111" s="10">
+        <v>0</v>
+      </c>
+      <c r="J111" s="9">
+        <f>I111*E111</f>
+        <v>0</v>
+      </c>
+      <c r="K111" s="3"/>
+    </row>
+    <row r="112" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+      <c r="A112" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="B111" s="3" t="s">
+      <c r="B112" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C111" s="3" t="s">
+      <c r="C112" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="D111" s="1" t="s">
+      <c r="D112" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="E111" s="3">
+      <c r="E112" s="3">
         <v>11.99</v>
-      </c>
-      <c r="G111" s="6">
-        <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
-      <c r="H111" s="3"/>
-      <c r="I111" s="8">
-        <v>0</v>
-      </c>
-      <c r="J111" s="9">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
-      <c r="K111" s="3"/>
-    </row>
-    <row r="112" spans="1:13" ht="105" x14ac:dyDescent="0.25">
-      <c r="A112" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="B112" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="C112" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D112" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="E112" s="3">
-        <v>32.880000000000003</v>
       </c>
       <c r="G112" s="6">
         <f t="shared" si="14"/>
@@ -5299,23 +5289,28 @@
       </c>
       <c r="K112" s="3"/>
     </row>
-    <row r="113" spans="1:11" ht="110.25" x14ac:dyDescent="0.25">
-      <c r="A113" s="14" t="s">
-        <v>232</v>
-      </c>
-      <c r="B113" s="14" t="s">
-        <v>233</v>
-      </c>
-      <c r="C113" s="14" t="s">
+    <row r="113" spans="1:11" ht="112" x14ac:dyDescent="0.2">
+      <c r="A113" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="B113" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="C113" s="3" t="s">
         <v>18</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="E113" s="14">
-        <v>12.99</v>
-      </c>
-      <c r="I113" s="3">
+        <v>105</v>
+      </c>
+      <c r="E113" s="3">
+        <v>32.880000000000003</v>
+      </c>
+      <c r="G113" s="6">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="H113" s="3"/>
+      <c r="I113" s="8">
         <v>0</v>
       </c>
       <c r="J113" s="9">
@@ -5324,73 +5319,73 @@
       </c>
       <c r="K113" s="3"/>
     </row>
-    <row r="114" spans="1:11" ht="105" x14ac:dyDescent="0.25">
-      <c r="A114" s="3" t="s">
-        <v>235</v>
+    <row r="114" spans="1:11" ht="85" x14ac:dyDescent="0.2">
+      <c r="A114" s="14" t="s">
+        <v>232</v>
       </c>
       <c r="B114" s="14" t="s">
-        <v>236</v>
-      </c>
-      <c r="C114" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D114" s="4" t="s">
-        <v>237</v>
-      </c>
-      <c r="E114" s="3">
-        <v>5.69</v>
+        <v>233</v>
+      </c>
+      <c r="C114" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="D114" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="E114" s="14">
+        <v>12.99</v>
       </c>
       <c r="I114" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J114" s="9">
         <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="K114" s="3"/>
+    </row>
+    <row r="115" spans="1:11" ht="176" x14ac:dyDescent="0.2">
+      <c r="A115" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="B115" s="14" t="s">
+        <v>236</v>
+      </c>
+      <c r="C115" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D115" s="4" t="s">
+        <v>237</v>
+      </c>
+      <c r="E115" s="3">
         <v>5.69</v>
       </c>
-      <c r="K114" s="21" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="115" spans="1:11" ht="75" x14ac:dyDescent="0.25">
-      <c r="A115" s="3" t="s">
-        <v>238</v>
-      </c>
-      <c r="B115" s="3" t="s">
-        <v>239</v>
-      </c>
-      <c r="C115" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D115" s="4" t="s">
-        <v>240</v>
-      </c>
-      <c r="E115" s="3">
-        <v>12</v>
-      </c>
       <c r="I115" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J115" s="9">
         <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
-      <c r="K115" s="3"/>
-    </row>
-    <row r="116" spans="1:11" ht="94.5" x14ac:dyDescent="0.25">
+        <v>5.69</v>
+      </c>
+      <c r="K115" s="21" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="116" spans="1:11" ht="80" x14ac:dyDescent="0.2">
       <c r="A116" s="3" t="s">
-        <v>241</v>
-      </c>
-      <c r="B116" s="14" t="s">
-        <v>242</v>
+        <v>238</v>
+      </c>
+      <c r="B116" s="3" t="s">
+        <v>239</v>
       </c>
       <c r="C116" s="3" t="s">
         <v>18</v>
       </c>
       <c r="D116" s="4" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="E116" s="3">
-        <v>8.99</v>
+        <v>12</v>
       </c>
       <c r="I116" s="3">
         <v>0</v>
@@ -5401,61 +5396,86 @@
       </c>
       <c r="K116" s="3"/>
     </row>
-    <row r="117" spans="1:11" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:11" ht="96" x14ac:dyDescent="0.2">
       <c r="A117" s="3" t="s">
-        <v>267</v>
+        <v>241</v>
       </c>
       <c r="B117" s="14" t="s">
-        <v>266</v>
+        <v>242</v>
       </c>
       <c r="C117" s="3" t="s">
         <v>18</v>
       </c>
       <c r="D117" s="4" t="s">
-        <v>268</v>
+        <v>243</v>
       </c>
       <c r="E117" s="3">
-        <v>19.989999999999998</v>
+        <v>8.99</v>
       </c>
       <c r="I117" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J117" s="9">
         <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="K117" s="3"/>
+    </row>
+    <row r="118" spans="1:11" ht="96" x14ac:dyDescent="0.2">
+      <c r="A118" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="B118" s="14" t="s">
+        <v>266</v>
+      </c>
+      <c r="C118" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D118" s="4" t="s">
+        <v>268</v>
+      </c>
+      <c r="E118" s="3">
         <v>19.989999999999998</v>
       </c>
-      <c r="K117" s="3"/>
+      <c r="I118" s="3">
+        <v>1</v>
+      </c>
+      <c r="J118" s="9">
+        <f t="shared" si="15"/>
+        <v>19.989999999999998</v>
+      </c>
+      <c r="K118" s="3"/>
     </row>
   </sheetData>
-  <autoFilter ref="A2:J117" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A60:J81">
-    <sortCondition ref="C60:C81"/>
+  <autoFilter ref="A2:J118" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A61:J82">
+    <sortCondition ref="C61:C82"/>
   </sortState>
   <hyperlinks>
     <hyperlink ref="D24" r:id="rId1" display="https://www.amazon.com/dp/B00LPK0E5A/ref=sspa_dk_detail_1?psc=1&amp;pd_rd_i=B00LPK0E5A&amp;pd_rd_w=0M9NZ&amp;pf_rd_p=48d372c1-f7e1-4b8b-9d02-4bd86f5158c5&amp;pd_rd_wg=aD93W&amp;pf_rd_r=YPJBQXW796NSXR2VMXXF&amp;pd_rd_r=27b44396-0b27-4df5-a333-c9ae450119d1&amp;spLa=ZW5jcnlwdGVkUXVhbGlmaWVyPUEzRjAzSlpTNDhOSDROJmVuY3J5cHRlZElkPUExMDI0NTg3UkZNOVI5WEJEMTBKJmVuY3J5cHRlZEFkSWQ9QTAwMTM0OTMxR1ZVVzZSMDhHUEYwJndpZGdldE5hbWU9c3BfZGV0YWlsJmFjdGlvbj1jbGlja1JlZGlyZWN0JmRvTm90TG9nQ2xpY2s9dHJ1ZQ==" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
-    <hyperlink ref="D69" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
-    <hyperlink ref="D66" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
+    <hyperlink ref="D70" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
+    <hyperlink ref="D67" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
     <hyperlink ref="D22" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
     <hyperlink ref="D21" r:id="rId5" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
     <hyperlink ref="D20" r:id="rId6" display="https://www.amazon.com/BOJACK-UA741General-Purpose-Operational-Amplifier/dp/B07WSB1VNH/ref=asc_df_B07WSB1VNH/?tag=hyprod-20&amp;linkCode=df0&amp;hvadid=416713541504&amp;hvpos=&amp;hvnetw=g&amp;hvrand=10187485487199424423&amp;hvpone=&amp;hvptwo=&amp;hvqmt=&amp;hvdev=c&amp;hvdvcmdl=&amp;hvlocint=&amp;hvlocphy=9030447&amp;hvtargid=pla-870040127419&amp;psc=1&amp;tag=&amp;ref=&amp;adgrpid=93604203773&amp;hvpone=&amp;hvptwo=&amp;hvadid=416713541504&amp;hvpos=&amp;hvnetw=g&amp;hvrand=10187485487199424423&amp;hvqmt=&amp;hvdev=c&amp;hvdvcmdl=&amp;hvlocint=&amp;hvlocphy=9030447&amp;hvtargid=pla-870040127419" xr:uid="{00000000-0004-0000-0100-000006000000}"/>
     <hyperlink ref="D19" r:id="rId7" display="https://www.amazon.com/LSR-Transistor-Assortment-Electronics-Electronic/dp/B07TV9FFFQ/ref=sr_1_1_sspa?dchild=1&amp;keywords=transistor+kit&amp;qid=1589997273&amp;sr=8-1-spons&amp;psc=1&amp;spLa=ZW5jcnlwdGVkUXVhbGlmaWVyPUEyNjRQNjZTRkNTMDBEJmVuY3J5cHRlZElkPUEwMjA2MDgzMTJBUTZXT1pMR1VFSyZlbmNyeXB0ZWRBZElkPUEwMzg4NDY4MzgxSDlaRERQMUxMQSZ3aWRnZXROYW1lPXNwX2F0ZiZhY3Rpb249Y2xpY2tSZWRpcmVjdCZkb05vdExvZ0NsaWNrPXRydWU=" xr:uid="{00000000-0004-0000-0100-000007000000}"/>
-    <hyperlink ref="D79" r:id="rId8" xr:uid="{00000000-0004-0000-0100-000008000000}"/>
-    <hyperlink ref="D68" r:id="rId9" xr:uid="{00000000-0004-0000-0100-000009000000}"/>
-    <hyperlink ref="D67" r:id="rId10" xr:uid="{00000000-0004-0000-0100-00000A000000}"/>
+    <hyperlink ref="D80" r:id="rId8" xr:uid="{00000000-0004-0000-0100-000008000000}"/>
+    <hyperlink ref="D69" r:id="rId9" xr:uid="{00000000-0004-0000-0100-000009000000}"/>
+    <hyperlink ref="D68" r:id="rId10" xr:uid="{00000000-0004-0000-0100-00000A000000}"/>
     <hyperlink ref="D25" r:id="rId11" display="https://www.amazon.com/Isopropyl-Alcohol-Grade-99-Anhydrous/dp/B01KK014F4/ref=asc_df_B01KK014F4/?tag=hyprod-20&amp;linkCode=df0&amp;hvadid=312416780110&amp;hvpos=&amp;hvnetw=g&amp;hvrand=17295135421118886149&amp;hvpone=&amp;hvptwo=&amp;hvqmt=&amp;hvdev=c&amp;hvdvcmdl=&amp;hvlocint=&amp;hvlocphy=9030447&amp;hvtargid=pla-569571734125&amp;psc=1&amp;tag=&amp;ref=&amp;adgrpid=61555869549&amp;hvpone=&amp;hvptwo=&amp;hvadid=312416780110&amp;hvpos=&amp;hvnetw=g&amp;hvrand=17295135421118886149&amp;hvqmt=&amp;hvdev=c&amp;hvdvcmdl=&amp;hvlocint=&amp;hvlocphy=9030447&amp;hvtargid=pla-569571734125" xr:uid="{00000000-0004-0000-0100-00000B000000}"/>
     <hyperlink ref="D29" r:id="rId12" xr:uid="{00000000-0004-0000-0100-00000C000000}"/>
     <hyperlink ref="D28" r:id="rId13" xr:uid="{00000000-0004-0000-0100-00000D000000}"/>
     <hyperlink ref="D18" r:id="rId14" xr:uid="{00000000-0004-0000-0100-00000E000000}"/>
-    <hyperlink ref="D106" r:id="rId15" xr:uid="{00000000-0004-0000-0100-00000F000000}"/>
+    <hyperlink ref="D107" r:id="rId15" xr:uid="{00000000-0004-0000-0100-00000F000000}"/>
     <hyperlink ref="D32" r:id="rId16" xr:uid="{00000000-0004-0000-0100-000010000000}"/>
     <hyperlink ref="D31" r:id="rId17" xr:uid="{00000000-0004-0000-0100-000011000000}"/>
     <hyperlink ref="D17" r:id="rId18" xr:uid="{00000000-0004-0000-0100-000012000000}"/>
     <hyperlink ref="D16" r:id="rId19" xr:uid="{00000000-0004-0000-0100-000013000000}"/>
     <hyperlink ref="D15" r:id="rId20" xr:uid="{00000000-0004-0000-0100-000014000000}"/>
-    <hyperlink ref="D105" r:id="rId21" xr:uid="{00000000-0004-0000-0100-000015000000}"/>
-    <hyperlink ref="D104" r:id="rId22" xr:uid="{00000000-0004-0000-0100-000016000000}"/>
-    <hyperlink ref="D62" r:id="rId23" display="https://www.amazon.com/Smart-Enabled-Google-Assistant-HomeKit/dp/B01NBI0A6R/ref=sxin_3_ac_d_rm?ac_md=0-0-d2Vtbw%3D%3D-ac_d_rm&amp;cv_ct_cx=wemo&amp;keywords=wemo&amp;pd_rd_i=B01NBI0A6R&amp;pd_rd_r=bbd5c2e2-6eb9-40fe-9456-a7336162120f&amp;pd_rd_w=Ts0oB&amp;pd_rd_wg=K1Zyb&amp;pf_rd_p=de19e82a-2d83-4ae8-9f5c-212586b8b9a0&amp;pf_rd_r=8DGZDACCDVJ418KR7CNJ&amp;qid=1584141937&amp;th=1" xr:uid="{00000000-0004-0000-0100-000017000000}"/>
-    <hyperlink ref="D61" r:id="rId24" xr:uid="{00000000-0004-0000-0100-000018000000}"/>
+    <hyperlink ref="D106" r:id="rId21" xr:uid="{00000000-0004-0000-0100-000015000000}"/>
+    <hyperlink ref="D105" r:id="rId22" xr:uid="{00000000-0004-0000-0100-000016000000}"/>
+    <hyperlink ref="D63" r:id="rId23" display="https://www.amazon.com/Smart-Enabled-Google-Assistant-HomeKit/dp/B01NBI0A6R/ref=sxin_3_ac_d_rm?ac_md=0-0-d2Vtbw%3D%3D-ac_d_rm&amp;cv_ct_cx=wemo&amp;keywords=wemo&amp;pd_rd_i=B01NBI0A6R&amp;pd_rd_r=bbd5c2e2-6eb9-40fe-9456-a7336162120f&amp;pd_rd_w=Ts0oB&amp;pd_rd_wg=K1Zyb&amp;pf_rd_p=de19e82a-2d83-4ae8-9f5c-212586b8b9a0&amp;pf_rd_r=8DGZDACCDVJ418KR7CNJ&amp;qid=1584141937&amp;th=1" xr:uid="{00000000-0004-0000-0100-000017000000}"/>
+    <hyperlink ref="D62" r:id="rId24" xr:uid="{00000000-0004-0000-0100-000018000000}"/>
     <hyperlink ref="D7" r:id="rId25" xr:uid="{00000000-0004-0000-0100-000019000000}"/>
     <hyperlink ref="D14" r:id="rId26" xr:uid="{00000000-0004-0000-0100-00001A000000}"/>
     <hyperlink ref="D27" r:id="rId27" xr:uid="{00000000-0004-0000-0100-00001B000000}"/>
@@ -5465,9 +5485,9 @@
     <hyperlink ref="D9" r:id="rId31" xr:uid="{00000000-0004-0000-0100-00001F000000}"/>
     <hyperlink ref="D8" r:id="rId32" xr:uid="{00000000-0004-0000-0100-000020000000}"/>
     <hyperlink ref="D11" r:id="rId33" xr:uid="{00000000-0004-0000-0100-000021000000}"/>
-    <hyperlink ref="B60" r:id="rId34" display="https://www.adafruit.com/product/1461" xr:uid="{00000000-0004-0000-0100-000022000000}"/>
-    <hyperlink ref="D110" r:id="rId35" xr:uid="{00000000-0004-0000-0100-000023000000}"/>
-    <hyperlink ref="D60" r:id="rId36" xr:uid="{00000000-0004-0000-0100-000024000000}"/>
+    <hyperlink ref="B61" r:id="rId34" display="https://www.adafruit.com/product/1461" xr:uid="{00000000-0004-0000-0100-000022000000}"/>
+    <hyperlink ref="D111" r:id="rId35" xr:uid="{00000000-0004-0000-0100-000023000000}"/>
+    <hyperlink ref="D61" r:id="rId36" xr:uid="{00000000-0004-0000-0100-000024000000}"/>
     <hyperlink ref="D3" r:id="rId37" xr:uid="{00000000-0004-0000-0100-000025000000}"/>
     <hyperlink ref="D35" r:id="rId38" xr:uid="{00000000-0004-0000-0100-000026000000}"/>
     <hyperlink ref="D34" r:id="rId39" xr:uid="{00000000-0004-0000-0100-000027000000}"/>
@@ -5477,48 +5497,48 @@
     <hyperlink ref="D13" r:id="rId43" xr:uid="{00000000-0004-0000-0100-00002B000000}"/>
     <hyperlink ref="D26" r:id="rId44" display="https://www.amazon.com/dp/B07GD2BWPY/ref=sspa_dk_detail_2?psc=1&amp;pd_rd_i=B07GD2BWPY&amp;pd_rd_w=TqeWX&amp;pf_rd_p=48d372c1-f7e1-4b8b-9d02-4bd86f5158c5&amp;pd_rd_wg=sNJWA&amp;pf_rd_r=ZXS16ECPMKD9XBVAS65W&amp;pd_rd_r=b5442918-7fb9-4962-af3b-9820970385cf&amp;spLa=ZW5jcnlwdGVkUXVhbGlmaWVyPUEyWTlUTDAyTTJDVElLJmVuY3J5cHRlZElkPUEwMjM2MDg0M0g1U1ZRS1hPNk0zMSZlbmNyeXB0ZWRBZElkPUEwNTczODQxM0JQVzgzUkcwMUVBNiZ3aWRnZXROYW1lPXNwX2RldGFpbCZhY3Rpb249Y2xpY2tSZWRpcmVjdCZkb05vdExvZ0NsaWNrPXRydWU=" xr:uid="{00000000-0004-0000-0100-00002C000000}"/>
     <hyperlink ref="D23" r:id="rId45" display="https://www.amazon.com/Qunqi-Sensor-Module-Arduino-Raspberry/dp/B07QBPGYBF/ref=pd_vtp_328_2/133-9447900-8990828?_encoding=UTF8&amp;pd_rd_i=B07QBPGYBF&amp;pd_rd_r=e7d105ef-e581-4e23-9137-ef46e7f59ac1&amp;pd_rd_w=4kywy&amp;pd_rd_wg=hamvp&amp;pf_rd_p=5946f538-3793-4aed-94d1-6882674b98f9&amp;pf_rd_r=V04NHSEY2AS5NV572E1P&amp;psc=1&amp;refRID=V04NHSEY2AS5NV572E1P" xr:uid="{00000000-0004-0000-0100-00002D000000}"/>
-    <hyperlink ref="D65" r:id="rId46" xr:uid="{00000000-0004-0000-0100-00002F000000}"/>
-    <hyperlink ref="D63" r:id="rId47" xr:uid="{00000000-0004-0000-0100-000030000000}"/>
-    <hyperlink ref="D108" r:id="rId48" display="https://www.amazon.com/Adafruit-NeoPixel-Ring-Integrated-Drivers/dp/B00KAE3R1U/ref=sxin_7_ac_d_rm?ac_md=1-1-bmVvcGl4ZWw%3D-ac_d_rm&amp;cv_ct_cx=neopixel+ring&amp;dchild=1&amp;keywords=neopixel+ring&amp;pd_rd_i=B00KAE3R1U&amp;pd_rd_r=f532ea9d-0030-44f0-832a-ce614c837962&amp;pd_rd_w=9bJ5n&amp;pd_rd_wg=0eBjE&amp;pf_rd_p=a0516f22-66df-4efd-8b9a-279a864d1512&amp;pf_rd_r=AYP2P98ZJBNCG2YYCT97&amp;psc=1&amp;qid=1590415826&amp;sr=1-2-12d4272d-8adb-4121-8624-135149aa9081" xr:uid="{00000000-0004-0000-0100-000031000000}"/>
-    <hyperlink ref="D111" r:id="rId49" xr:uid="{00000000-0004-0000-0100-000032000000}"/>
-    <hyperlink ref="D112" r:id="rId50" display="https://www.amazon.com/dp/B01CDTEKAG/ref=sspa_dk_detail_5?psc=1&amp;pd_rd_i=B01CDTEKAG&amp;pd_rd_w=xH4vG&amp;pf_rd_p=48d372c1-f7e1-4b8b-9d02-4bd86f5158c5&amp;pd_rd_wg=OWknK&amp;pf_rd_r=4MWDRWVKFJB1AYRB3KT5&amp;pd_rd_r=1dfe850a-4ea2-46f2-b93c-46b84486f9d4&amp;spLa=ZW5jcnlwdGVkUXVhbGlmaWVyPUEzUThIV0Y2UjRSUjImZW5jcnlwdGVkSWQ9QTAzMjQ0ODUxSDdUU0E3UTlMWFlEJmVuY3J5cHRlZEFkSWQ9QTA5Nzg1MTUxVTM3VzVKSE44S1RCJndpZGdldE5hbWU9c3BfZGV0YWlsJmFjdGlvbj1jbGlja1JlZGlyZWN0JmRvTm90TG9nQ2xpY2s9dHJ1ZQ==" xr:uid="{00000000-0004-0000-0100-000033000000}"/>
-    <hyperlink ref="D80" r:id="rId51" display="https://www.amazon.com/DFROBOT-Gravity-Analog-Sensor-Arduino/dp/B00R5CCH7U/ref=sr_1_2_sspa?dchild=1&amp;keywords=dfrobot&amp;qid=1590416675&amp;sr=8-2-spons&amp;psc=1&amp;spLa=ZW5jcnlwdGVkUXVhbGlmaWVyPUExRVhTUks4U1dYNjhSJmVuY3J5cHRlZElkPUEwNTY0MzYzUldBQ1A2SDlRVkRCJmVuY3J5cHRlZEFkSWQ9QTEwNDU4OTYzVjNDWEhNV0RPS1IzJndpZGdldE5hbWU9c3BfYXRmJmFjdGlvbj1jbGlja1JlZGlyZWN0JmRvTm90TG9nQ2xpY2s9dHJ1ZQ==" xr:uid="{00000000-0004-0000-0100-000034000000}"/>
-    <hyperlink ref="D77" r:id="rId52" xr:uid="{00000000-0004-0000-0100-000035000000}"/>
-    <hyperlink ref="D78" r:id="rId53" xr:uid="{00000000-0004-0000-0100-000036000000}"/>
-    <hyperlink ref="D73" r:id="rId54" xr:uid="{00000000-0004-0000-0100-000037000000}"/>
-    <hyperlink ref="D71" r:id="rId55" xr:uid="{00000000-0004-0000-0100-000038000000}"/>
+    <hyperlink ref="D66" r:id="rId46" xr:uid="{00000000-0004-0000-0100-00002F000000}"/>
+    <hyperlink ref="D64" r:id="rId47" xr:uid="{00000000-0004-0000-0100-000030000000}"/>
+    <hyperlink ref="D109" r:id="rId48" display="https://www.amazon.com/Adafruit-NeoPixel-Ring-Integrated-Drivers/dp/B00KAE3R1U/ref=sxin_7_ac_d_rm?ac_md=1-1-bmVvcGl4ZWw%3D-ac_d_rm&amp;cv_ct_cx=neopixel+ring&amp;dchild=1&amp;keywords=neopixel+ring&amp;pd_rd_i=B00KAE3R1U&amp;pd_rd_r=f532ea9d-0030-44f0-832a-ce614c837962&amp;pd_rd_w=9bJ5n&amp;pd_rd_wg=0eBjE&amp;pf_rd_p=a0516f22-66df-4efd-8b9a-279a864d1512&amp;pf_rd_r=AYP2P98ZJBNCG2YYCT97&amp;psc=1&amp;qid=1590415826&amp;sr=1-2-12d4272d-8adb-4121-8624-135149aa9081" xr:uid="{00000000-0004-0000-0100-000031000000}"/>
+    <hyperlink ref="D112" r:id="rId49" xr:uid="{00000000-0004-0000-0100-000032000000}"/>
+    <hyperlink ref="D113" r:id="rId50" display="https://www.amazon.com/dp/B01CDTEKAG/ref=sspa_dk_detail_5?psc=1&amp;pd_rd_i=B01CDTEKAG&amp;pd_rd_w=xH4vG&amp;pf_rd_p=48d372c1-f7e1-4b8b-9d02-4bd86f5158c5&amp;pd_rd_wg=OWknK&amp;pf_rd_r=4MWDRWVKFJB1AYRB3KT5&amp;pd_rd_r=1dfe850a-4ea2-46f2-b93c-46b84486f9d4&amp;spLa=ZW5jcnlwdGVkUXVhbGlmaWVyPUEzUThIV0Y2UjRSUjImZW5jcnlwdGVkSWQ9QTAzMjQ0ODUxSDdUU0E3UTlMWFlEJmVuY3J5cHRlZEFkSWQ9QTA5Nzg1MTUxVTM3VzVKSE44S1RCJndpZGdldE5hbWU9c3BfZGV0YWlsJmFjdGlvbj1jbGlja1JlZGlyZWN0JmRvTm90TG9nQ2xpY2s9dHJ1ZQ==" xr:uid="{00000000-0004-0000-0100-000033000000}"/>
+    <hyperlink ref="D81" r:id="rId51" display="https://www.amazon.com/DFROBOT-Gravity-Analog-Sensor-Arduino/dp/B00R5CCH7U/ref=sr_1_2_sspa?dchild=1&amp;keywords=dfrobot&amp;qid=1590416675&amp;sr=8-2-spons&amp;psc=1&amp;spLa=ZW5jcnlwdGVkUXVhbGlmaWVyPUExRVhTUks4U1dYNjhSJmVuY3J5cHRlZElkPUEwNTY0MzYzUldBQ1A2SDlRVkRCJmVuY3J5cHRlZEFkSWQ9QTEwNDU4OTYzVjNDWEhNV0RPS1IzJndpZGdldE5hbWU9c3BfYXRmJmFjdGlvbj1jbGlja1JlZGlyZWN0JmRvTm90TG9nQ2xpY2s9dHJ1ZQ==" xr:uid="{00000000-0004-0000-0100-000034000000}"/>
+    <hyperlink ref="D78" r:id="rId52" xr:uid="{00000000-0004-0000-0100-000035000000}"/>
+    <hyperlink ref="D79" r:id="rId53" xr:uid="{00000000-0004-0000-0100-000036000000}"/>
+    <hyperlink ref="D74" r:id="rId54" xr:uid="{00000000-0004-0000-0100-000037000000}"/>
+    <hyperlink ref="D72" r:id="rId55" xr:uid="{00000000-0004-0000-0100-000038000000}"/>
     <hyperlink ref="D38" r:id="rId56" display="https://www.lowes.com/pd/Tough-Box-16-Compartment-Plastic-Small-Parts-Organizer/1000365903?cm_mmc=shp-_-c-_-prd-_-tol-_-google-_-lia-_--_-toolstorage-_-1000365903-_-0&amp;store_code=2539&amp;placeholder=null&amp;gclid=EAIaIQobChMI2ICzhsX86QIVi4bACh0oNwjhEAQYASABEgLcgPD_BwE&amp;gclsrc=aw.ds" xr:uid="{00000000-0004-0000-0100-00003B000000}"/>
-    <hyperlink ref="D81" r:id="rId57" xr:uid="{00000000-0004-0000-0100-00003C000000}"/>
-    <hyperlink ref="D82" r:id="rId58" xr:uid="{00000000-0004-0000-0100-00003D000000}"/>
-    <hyperlink ref="D83" r:id="rId59" xr:uid="{00000000-0004-0000-0100-00003E000000}"/>
-    <hyperlink ref="D113" r:id="rId60" display="https://www.amazon.com/dp/B087B5NWY4/ref=sspa_dk_detail_0?psc=1&amp;pd_rd_i=B087B5NWY4&amp;pd_rd_w=qTl74&amp;pf_rd_p=48d372c1-f7e1-4b8b-9d02-4bd86f5158c5&amp;pd_rd_wg=oJf3C&amp;pf_rd_r=BNJEBNTQ9WJFCK2T7NJG&amp;pd_rd_r=878dff4d-97fc-4ab7-b51d-f454e436af7d&amp;spLa=ZW5jcnlwdGVkUXVhbGlmaWVyPUFSMFdOVFk0RUJCSjUmZW5jcnlwdGVkSWQ9QTA5OTM1MjYzSTlCWEhXN0xTU0RQJmVuY3J5cHRlZEFkSWQ9QTAxMzk3MzYzQktQVENFTUtJNzhJJndpZGdldE5hbWU9c3BfZGV0YWlsJmFjdGlvbj1jbGlja1JlZGlyZWN0JmRvTm90TG9nQ2xpY2s9dHJ1ZQ==" xr:uid="{00000000-0004-0000-0100-00003F000000}"/>
+    <hyperlink ref="D82" r:id="rId57" xr:uid="{00000000-0004-0000-0100-00003C000000}"/>
+    <hyperlink ref="D83" r:id="rId58" xr:uid="{00000000-0004-0000-0100-00003D000000}"/>
+    <hyperlink ref="D84" r:id="rId59" xr:uid="{00000000-0004-0000-0100-00003E000000}"/>
+    <hyperlink ref="D114" r:id="rId60" display="https://www.amazon.com/dp/B087B5NWY4/ref=sspa_dk_detail_0?psc=1&amp;pd_rd_i=B087B5NWY4&amp;pd_rd_w=qTl74&amp;pf_rd_p=48d372c1-f7e1-4b8b-9d02-4bd86f5158c5&amp;pd_rd_wg=oJf3C&amp;pf_rd_r=BNJEBNTQ9WJFCK2T7NJG&amp;pd_rd_r=878dff4d-97fc-4ab7-b51d-f454e436af7d&amp;spLa=ZW5jcnlwdGVkUXVhbGlmaWVyPUFSMFdOVFk0RUJCSjUmZW5jcnlwdGVkSWQ9QTA5OTM1MjYzSTlCWEhXN0xTU0RQJmVuY3J5cHRlZEFkSWQ9QTAxMzk3MzYzQktQVENFTUtJNzhJJndpZGdldE5hbWU9c3BfZGV0YWlsJmFjdGlvbj1jbGlja1JlZGlyZWN0JmRvTm90TG9nQ2xpY2s9dHJ1ZQ==" xr:uid="{00000000-0004-0000-0100-00003F000000}"/>
     <hyperlink ref="D39" r:id="rId61" xr:uid="{00000000-0004-0000-0100-000040000000}"/>
-    <hyperlink ref="D84" r:id="rId62" xr:uid="{00000000-0004-0000-0100-000041000000}"/>
-    <hyperlink ref="D85" r:id="rId63" xr:uid="{00000000-0004-0000-0100-000042000000}"/>
-    <hyperlink ref="D86" r:id="rId64" xr:uid="{00000000-0004-0000-0100-000043000000}"/>
-    <hyperlink ref="D114" r:id="rId65" display="https://www.amazon.com/dp/B07QKDSCSM/ref=sspa_dk_detail_0?spLa=ZW5jcnlwdGVkUXVhbGlmaWVyPUFCNUFXNjBMUkhRNjgmZW5jcnlwdGVkSWQ9QTAzODUwNTVOR1NCNFFLMjRWR0ImZW5jcnlwdGVkQWRJZD1BMDM1MDc1NjNWSVJZSlg1Q0pDTUkmd2lkZ2V0TmFtZT1zcF9kZXRhaWwyJmFjdGlvbj1jbGlja1JlZGlyZWN0JmRvTm90TG9nQ2xpY2s9dHJ1ZQ&amp;th=1" xr:uid="{00000000-0004-0000-0100-000044000000}"/>
-    <hyperlink ref="D90" r:id="rId66" xr:uid="{00000000-0004-0000-0100-000045000000}"/>
-    <hyperlink ref="D91" r:id="rId67" xr:uid="{00000000-0004-0000-0100-000046000000}"/>
-    <hyperlink ref="D116" r:id="rId68" xr:uid="{00000000-0004-0000-0100-000047000000}"/>
-    <hyperlink ref="D115" r:id="rId69" xr:uid="{00000000-0004-0000-0100-000048000000}"/>
-    <hyperlink ref="D92" r:id="rId70" display="https://www.digikey.com/product-detail/en/citizen-finedevice-co-ltd/CFS-20632768DZFB/300-1002-ND/283736?utm_adgroup=Crystals%20Oscillators&amp;utm_source=google&amp;utm_medium=cpc&amp;utm_campaign=Dynamic%20Search&amp;utm_term=&amp;utm_content=Crystals%20Oscillators&amp;gclid=EAIaIQobChMIrI-y8dvf6gIVgobACh05Cwq-EAAYASAAEgJ-LvD_BwE" xr:uid="{00000000-0004-0000-0100-00004A000000}"/>
-    <hyperlink ref="D72" r:id="rId71" xr:uid="{00000000-0004-0000-0100-00004B000000}"/>
-    <hyperlink ref="D74" r:id="rId72" xr:uid="{00000000-0004-0000-0100-00004C000000}"/>
-    <hyperlink ref="D75" r:id="rId73" xr:uid="{00000000-0004-0000-0100-00004D000000}"/>
-    <hyperlink ref="D76" r:id="rId74" xr:uid="{00000000-0004-0000-0100-00004E000000}"/>
-    <hyperlink ref="B70" r:id="rId75" display="https://store.ncd.io/product/feather-battery-i2c-shield-for-particle-and-feather-modules/" xr:uid="{00000000-0004-0000-0100-00003A000000}"/>
-    <hyperlink ref="D70" r:id="rId76" xr:uid="{00000000-0004-0000-0100-000039000000}"/>
-    <hyperlink ref="D87" r:id="rId77" xr:uid="{CB9AA7F3-57D3-4035-9B10-D6E06BA90642}"/>
-    <hyperlink ref="D88" r:id="rId78" xr:uid="{CD5B5197-64EF-49EF-91BD-2559DCFA1A39}"/>
-    <hyperlink ref="D89" r:id="rId79" xr:uid="{6673B4F9-7D5C-42C3-A449-534270670C62}"/>
-    <hyperlink ref="D93" r:id="rId80" xr:uid="{7BEE6173-67BD-462D-93F3-8868348A9E43}"/>
-    <hyperlink ref="D95" r:id="rId81" display="https://www.amazon.com/Screwdriver-Flathead-Phillips-Pentalobe-Different/dp/B0872XMTKS/ref=sr_1_2_sspa?crid=33O94WILFA3IZ&amp;dchild=1&amp;keywords=mini+screwdriver+set&amp;qid=1598205307&amp;sprefix=mini+screw%2Caps%2C201&amp;sr=8-2-spons&amp;psc=1&amp;spLa=ZW5jcnlwdGVkUXVhbGlmaWVyPUExMEY2S0QwRE9XR01UJmVuY3J5cHRlZElkPUEwNzIwODY1MjVGV1BCNDNFNkowRyZlbmNyeXB0ZWRBZElkPUExMDAyMjM5NFpSMkVPTlBSN0ZDJndpZGdldE5hbWU9c3BfYXRmJmFjdGlvbj1jbGlja1JlZGlyZWN0JmRvTm90TG9nQ2xpY2s9dHJ1ZQ==" xr:uid="{19DAF842-E937-4DB9-89CA-2282F04D2AEA}"/>
+    <hyperlink ref="D85" r:id="rId62" xr:uid="{00000000-0004-0000-0100-000041000000}"/>
+    <hyperlink ref="D86" r:id="rId63" xr:uid="{00000000-0004-0000-0100-000042000000}"/>
+    <hyperlink ref="D87" r:id="rId64" xr:uid="{00000000-0004-0000-0100-000043000000}"/>
+    <hyperlink ref="D115" r:id="rId65" display="https://www.amazon.com/dp/B07QKDSCSM/ref=sspa_dk_detail_0?spLa=ZW5jcnlwdGVkUXVhbGlmaWVyPUFCNUFXNjBMUkhRNjgmZW5jcnlwdGVkSWQ9QTAzODUwNTVOR1NCNFFLMjRWR0ImZW5jcnlwdGVkQWRJZD1BMDM1MDc1NjNWSVJZSlg1Q0pDTUkmd2lkZ2V0TmFtZT1zcF9kZXRhaWwyJmFjdGlvbj1jbGlja1JlZGlyZWN0JmRvTm90TG9nQ2xpY2s9dHJ1ZQ&amp;th=1" xr:uid="{00000000-0004-0000-0100-000044000000}"/>
+    <hyperlink ref="D91" r:id="rId66" xr:uid="{00000000-0004-0000-0100-000045000000}"/>
+    <hyperlink ref="D92" r:id="rId67" xr:uid="{00000000-0004-0000-0100-000046000000}"/>
+    <hyperlink ref="D117" r:id="rId68" xr:uid="{00000000-0004-0000-0100-000047000000}"/>
+    <hyperlink ref="D116" r:id="rId69" xr:uid="{00000000-0004-0000-0100-000048000000}"/>
+    <hyperlink ref="D93" r:id="rId70" display="https://www.digikey.com/product-detail/en/citizen-finedevice-co-ltd/CFS-20632768DZFB/300-1002-ND/283736?utm_adgroup=Crystals%20Oscillators&amp;utm_source=google&amp;utm_medium=cpc&amp;utm_campaign=Dynamic%20Search&amp;utm_term=&amp;utm_content=Crystals%20Oscillators&amp;gclid=EAIaIQobChMIrI-y8dvf6gIVgobACh05Cwq-EAAYASAAEgJ-LvD_BwE" xr:uid="{00000000-0004-0000-0100-00004A000000}"/>
+    <hyperlink ref="D73" r:id="rId71" xr:uid="{00000000-0004-0000-0100-00004B000000}"/>
+    <hyperlink ref="D75" r:id="rId72" xr:uid="{00000000-0004-0000-0100-00004C000000}"/>
+    <hyperlink ref="D76" r:id="rId73" xr:uid="{00000000-0004-0000-0100-00004D000000}"/>
+    <hyperlink ref="D77" r:id="rId74" xr:uid="{00000000-0004-0000-0100-00004E000000}"/>
+    <hyperlink ref="B71" r:id="rId75" display="https://store.ncd.io/product/feather-battery-i2c-shield-for-particle-and-feather-modules/" xr:uid="{00000000-0004-0000-0100-00003A000000}"/>
+    <hyperlink ref="D71" r:id="rId76" xr:uid="{00000000-0004-0000-0100-000039000000}"/>
+    <hyperlink ref="D88" r:id="rId77" xr:uid="{CB9AA7F3-57D3-4035-9B10-D6E06BA90642}"/>
+    <hyperlink ref="D89" r:id="rId78" xr:uid="{CD5B5197-64EF-49EF-91BD-2559DCFA1A39}"/>
+    <hyperlink ref="D90" r:id="rId79" xr:uid="{6673B4F9-7D5C-42C3-A449-534270670C62}"/>
+    <hyperlink ref="D94" r:id="rId80" xr:uid="{7BEE6173-67BD-462D-93F3-8868348A9E43}"/>
+    <hyperlink ref="D96" r:id="rId81" display="https://www.amazon.com/Screwdriver-Flathead-Phillips-Pentalobe-Different/dp/B0872XMTKS/ref=sr_1_2_sspa?crid=33O94WILFA3IZ&amp;dchild=1&amp;keywords=mini+screwdriver+set&amp;qid=1598205307&amp;sprefix=mini+screw%2Caps%2C201&amp;sr=8-2-spons&amp;psc=1&amp;spLa=ZW5jcnlwdGVkUXVhbGlmaWVyPUExMEY2S0QwRE9XR01UJmVuY3J5cHRlZElkPUEwNzIwODY1MjVGV1BCNDNFNkowRyZlbmNyeXB0ZWRBZElkPUExMDAyMjM5NFpSMkVPTlBSN0ZDJndpZGdldE5hbWU9c3BfYXRmJmFjdGlvbj1jbGlja1JlZGlyZWN0JmRvTm90TG9nQ2xpY2s9dHJ1ZQ==" xr:uid="{19DAF842-E937-4DB9-89CA-2282F04D2AEA}"/>
     <hyperlink ref="D40" r:id="rId82" xr:uid="{B485A6B6-7307-4EAA-A186-31CAA890A0BC}"/>
-    <hyperlink ref="D107" r:id="rId83" xr:uid="{70F21853-AE4C-4BEC-9F14-C2DC1DDCC3B4}"/>
-    <hyperlink ref="D117" r:id="rId84" xr:uid="{23C2A1DE-EDE1-4FE6-90BB-24BA9B7A433E}"/>
+    <hyperlink ref="D108" r:id="rId83" xr:uid="{70F21853-AE4C-4BEC-9F14-C2DC1DDCC3B4}"/>
+    <hyperlink ref="D118" r:id="rId84" xr:uid="{23C2A1DE-EDE1-4FE6-90BB-24BA9B7A433E}"/>
     <hyperlink ref="D33" r:id="rId85" xr:uid="{AA5B840A-EAA7-438B-AC90-9BD9F369A790}"/>
-    <hyperlink ref="D109" r:id="rId86" xr:uid="{BFF0F66D-BAE5-409E-9D4D-2406089A97E9}"/>
-    <hyperlink ref="D45" r:id="rId87" xr:uid="{E22E05A0-7702-4DD5-A4C2-BD50049E3BED}"/>
+    <hyperlink ref="D110" r:id="rId86" xr:uid="{BFF0F66D-BAE5-409E-9D4D-2406089A97E9}"/>
+    <hyperlink ref="D46" r:id="rId87" xr:uid="{E22E05A0-7702-4DD5-A4C2-BD50049E3BED}"/>
   </hyperlinks>
   <printOptions headings="1" gridLines="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5748,18 +5768,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5782,18 +5802,18 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{58CD0F9C-796C-40DA-891C-7A92FF34C67A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{623B2E16-5227-4FB6-A3C3-1FFAD3C257CB}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{58CD0F9C-796C-40DA-891C-7A92FF34C67A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>